<commit_message>
Insert check sheet name in write to excel
</commit_message>
<xml_diff>
--- a/pendulum/work_on_memory/memory_grav.xlsx
+++ b/pendulum/work_on_memory/memory_grav.xlsx
@@ -8,18 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sky/Documents/Work Info/Research Assistant/deap_experiments/pendulum/work_on_memory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{660FBA30-E2C8-C84B-9AFF-B08DB88771B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7AD94E-05DA-094B-9C23-2D5D504C23F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15680" xr2:uid="{FC52945D-DEF3-A340-A70E-E7CD570E6620}"/>
+    <workbookView xWindow="5600" yWindow="2320" windowWidth="28040" windowHeight="15680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -36,9 +33,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>empty</t>
+    <t>sub(read(a0, a1), add(add(add(a2, a2), a2), add(a2, add(add(a2, write(a0, sin(0), add(sin(read(a0, limit(a2, protectedLog(a2), a2))), a2))), add(a2, sub(protectedDiv(abs(a2), a2), read(a0, read(a0, cos(conditional(a1, 0))))))))))</t>
+  </si>
+  <si>
+    <t>protectedDiv(add(read(a0, read(a0, sub(sin(add(read(a0, a1), protectedDiv(0, a1))), protectedDiv(0, a2)))), a2), conditional(sin(sin(read(a0, a1))), write(a0, limit(protectedLog(read(a0, add(add(conditional(abs(sin(a1)), a1), a2), sin(sin(a2))))), abs(limit(0, read(a0, a2), 0)), conditional(protectedDiv(0, a1), protectedDiv(a1, conditional(a2, read(a0, 0))))), a2)))</t>
+  </si>
+  <si>
+    <t>sub(sub(limit(a2, read(a0, a2), protectedLog(read(a0, abs(0)))), a2), add(write(a0, protectedLog(sub(conditional(a1, a2), sin(a2))), write(a0, protectedDiv(a1, limit(0, 0, limit(write(a0, a1, write(a0, 0, a2)), a2, a2))), a2)), limit(sin(cos(sub(protectedLog(abs(a2)), a2))), sub(0, limit(a2, a1, 0)), a2)))</t>
+  </si>
+  <si>
+    <t>sub(sub(read(a0, a1), add(write(a0, abs(a2), protectedDiv(add(a2, a2), protectedLog(write(a0, sin(cos(0)), abs(a1))))), cos(read(a0, read(a0, abs(sub(a1, conditional(limit(a2, limit(0, a1, a2), a2), a1)))))))), sub(a2, protectedLog(a2)))</t>
+  </si>
+  <si>
+    <t>sub(read(a0, a2), write(a0, sub(conditional(write(a0, a1, protectedLog(conditional(a1, protectedLog(a1)))), add(abs(0), sub(abs(write(a0, a1, a1)), add(protectedDiv(a2, a2), limit(0, 0, 0))))), conditional(0, conditional(conditional(a2, abs(a1)), a1))), protectedDiv(a2, conditional(sub(a2, sin(sin(write(a0, abs(conditional(sin(a1), 0)), a2)))), a2))))</t>
+  </si>
+  <si>
+    <t>sub(sub(0, read(a0, a1)), add(protectedDiv(conditional(a2, read(a0, read(a0, a1))), a2), add(write(a0, a1, sin(a2)), a2)))</t>
+  </si>
+  <si>
+    <t>sub(protectedDiv(sub(protectedDiv(conditional(read(a0, a2), a2), a2), sin(limit(0, 0, a1))), cos(sub(write(a0, 0, a2), cos(limit(cos(sin(a2)), 0, read(a0, 0)))))), a2)</t>
+  </si>
+  <si>
+    <t>sub(sub(read(a0, 0), protectedDiv(limit(sin(a1), protectedDiv(a2, protectedDiv(read(a0, a2), a1)), protectedLog(read(a0, a2))), a2)), write(a0, a2, a2))</t>
+  </si>
+  <si>
+    <t>protectedDiv(sub(sub(0, write(a0, a2, conditional(conditional(a2, 0), sin(read(a0, 0))))), write(a0, protectedDiv(a1, a1), conditional(conditional(a2, 0), read(a0, 0)))), a2)</t>
+  </si>
+  <si>
+    <t>Ind</t>
   </si>
 </sst>
 </file>
@@ -389,18 +413,609 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A45673E-47AF-C040-8EF2-4E9D430DC839}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9.81</v>
+      </c>
+      <c r="K1">
+        <v>11</v>
+      </c>
+      <c r="L1">
+        <v>12</v>
+      </c>
+      <c r="M1">
+        <v>13</v>
+      </c>
+      <c r="N1">
+        <v>14</v>
+      </c>
+      <c r="O1">
+        <v>15</v>
+      </c>
+      <c r="P1">
+        <v>16</v>
+      </c>
+      <c r="Q1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>0</v>
+      </c>
+      <c r="B2">
+        <v>-275.23</v>
+      </c>
+      <c r="C2">
+        <v>-242.91</v>
+      </c>
+      <c r="D2">
+        <v>-134.72</v>
+      </c>
+      <c r="E2">
+        <v>-150.97999999999999</v>
+      </c>
+      <c r="F2">
+        <v>-815.37</v>
+      </c>
+      <c r="G2">
+        <v>-700.74</v>
+      </c>
+      <c r="H2">
+        <v>-709.36</v>
+      </c>
+      <c r="I2">
+        <v>-682.57</v>
+      </c>
+      <c r="J2">
+        <v>-913.48</v>
+      </c>
+      <c r="K2">
+        <v>-948.93</v>
+      </c>
+      <c r="L2">
+        <v>-1148.8800000000001</v>
+      </c>
+      <c r="M2">
+        <v>-1135.3</v>
+      </c>
+      <c r="N2">
+        <v>-1295.02</v>
+      </c>
+      <c r="O2">
+        <v>-1344.59</v>
+      </c>
+      <c r="P2">
+        <v>-1539.4</v>
+      </c>
+      <c r="Q2">
+        <v>-1694.02</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>-63.71</v>
+      </c>
+      <c r="C3">
+        <v>-79.34</v>
+      </c>
+      <c r="D3">
+        <v>-71.709999999999994</v>
+      </c>
+      <c r="E3">
+        <v>-107.46</v>
+      </c>
+      <c r="F3">
+        <v>-662.35</v>
+      </c>
+      <c r="G3">
+        <v>-360.37</v>
+      </c>
+      <c r="H3">
+        <v>-363.8</v>
+      </c>
+      <c r="I3">
+        <v>-338.91</v>
+      </c>
+      <c r="J3">
+        <v>-351.74</v>
+      </c>
+      <c r="K3">
+        <v>-740.29</v>
+      </c>
+      <c r="L3">
+        <v>-729.01</v>
+      </c>
+      <c r="M3">
+        <v>-964.33</v>
+      </c>
+      <c r="N3">
+        <v>-826.55</v>
+      </c>
+      <c r="O3">
+        <v>-1287.4100000000001</v>
+      </c>
+      <c r="P3">
+        <v>-1439.09</v>
+      </c>
+      <c r="Q3">
+        <v>-1654.47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>-261.11</v>
+      </c>
+      <c r="C4">
+        <v>-259.39999999999998</v>
+      </c>
+      <c r="D4">
+        <v>-232.87</v>
+      </c>
+      <c r="E4">
+        <v>-482.79</v>
+      </c>
+      <c r="F4">
+        <v>-496.35</v>
+      </c>
+      <c r="G4">
+        <v>-447.32</v>
+      </c>
+      <c r="H4">
+        <v>-482.08</v>
+      </c>
+      <c r="I4">
+        <v>-662.74</v>
+      </c>
+      <c r="J4">
+        <v>-831.64</v>
+      </c>
+      <c r="K4">
+        <v>-965.16</v>
+      </c>
+      <c r="L4">
+        <v>-1043.54</v>
+      </c>
+      <c r="M4">
+        <v>-1173.49</v>
+      </c>
+      <c r="N4">
+        <v>-1281.57</v>
+      </c>
+      <c r="O4">
+        <v>-1170.3699999999999</v>
+      </c>
+      <c r="P4">
+        <v>-1585.31</v>
+      </c>
+      <c r="Q4">
+        <v>-1700.21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>-122.45</v>
+      </c>
+      <c r="C5">
+        <v>-188.19</v>
+      </c>
+      <c r="D5">
+        <v>-313.43</v>
+      </c>
+      <c r="E5">
+        <v>-320.75</v>
+      </c>
+      <c r="F5">
+        <v>-442.52</v>
+      </c>
+      <c r="G5">
+        <v>-421.35</v>
+      </c>
+      <c r="H5">
+        <v>-356.11</v>
+      </c>
+      <c r="I5">
+        <v>-345.63</v>
+      </c>
+      <c r="J5">
+        <v>-303.81</v>
+      </c>
+      <c r="K5">
+        <v>-322.44</v>
+      </c>
+      <c r="L5">
+        <v>-440.37</v>
+      </c>
+      <c r="M5">
+        <v>-1043.8900000000001</v>
+      </c>
+      <c r="N5">
+        <v>-1538.81</v>
+      </c>
+      <c r="O5">
+        <v>-1513.8</v>
+      </c>
+      <c r="P5">
+        <v>-1678.98</v>
+      </c>
+      <c r="Q5">
+        <v>-1853.78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>-1058.8599999999999</v>
+      </c>
+      <c r="C6">
+        <v>-1048.5</v>
+      </c>
+      <c r="D6">
+        <v>-1014.58</v>
+      </c>
+      <c r="E6">
+        <v>-1044.93</v>
+      </c>
+      <c r="F6">
+        <v>-1054.05</v>
+      </c>
+      <c r="G6">
+        <v>-1071.25</v>
+      </c>
+      <c r="H6">
+        <v>-952.87</v>
+      </c>
+      <c r="I6">
+        <v>-742.33</v>
+      </c>
+      <c r="J6">
+        <v>-612.87</v>
+      </c>
+      <c r="K6">
+        <v>-1153.49</v>
+      </c>
+      <c r="L6">
+        <v>-1467.79</v>
+      </c>
+      <c r="M6">
+        <v>-1598.73</v>
+      </c>
+      <c r="N6">
+        <v>-1752.86</v>
+      </c>
+      <c r="O6">
+        <v>-1846.33</v>
+      </c>
+      <c r="P6">
+        <v>-1944.15</v>
+      </c>
+      <c r="Q6">
+        <v>-2005.55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>-102.45</v>
+      </c>
+      <c r="C7">
+        <v>-79.069999999999993</v>
+      </c>
+      <c r="D7">
+        <v>-74.41</v>
+      </c>
+      <c r="E7">
+        <v>-117.78</v>
+      </c>
+      <c r="F7">
+        <v>-501.02</v>
+      </c>
+      <c r="G7">
+        <v>-306.77999999999997</v>
+      </c>
+      <c r="H7">
+        <v>-426.89</v>
+      </c>
+      <c r="I7">
+        <v>-289.20999999999998</v>
+      </c>
+      <c r="J7">
+        <v>-327.29000000000002</v>
+      </c>
+      <c r="K7">
+        <v>-568.05999999999995</v>
+      </c>
+      <c r="L7">
+        <v>-650.11</v>
+      </c>
+      <c r="M7">
+        <v>-758.64</v>
+      </c>
+      <c r="N7">
+        <v>-882.11</v>
+      </c>
+      <c r="O7">
+        <v>-915.95</v>
+      </c>
+      <c r="P7">
+        <v>-1393.81</v>
+      </c>
+      <c r="Q7">
+        <v>-1571.79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>-506.76</v>
+      </c>
+      <c r="C8">
+        <v>-813.67</v>
+      </c>
+      <c r="D8">
+        <v>-880.16</v>
+      </c>
+      <c r="E8">
+        <v>-938.72</v>
+      </c>
+      <c r="F8">
+        <v>-764.31</v>
+      </c>
+      <c r="G8">
+        <v>-683.06</v>
+      </c>
+      <c r="H8">
+        <v>-559.30999999999995</v>
+      </c>
+      <c r="I8">
+        <v>-769.61</v>
+      </c>
+      <c r="J8">
+        <v>-845.07</v>
+      </c>
+      <c r="K8">
+        <v>-890.64</v>
+      </c>
+      <c r="L8">
+        <v>-1367.43</v>
+      </c>
+      <c r="M8">
+        <v>-1567.2</v>
+      </c>
+      <c r="N8">
+        <v>-1690.3</v>
+      </c>
+      <c r="O8">
+        <v>-1772.79</v>
+      </c>
+      <c r="P8">
+        <v>-1895.94</v>
+      </c>
+      <c r="Q8">
+        <v>-1972.24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>-253.51</v>
+      </c>
+      <c r="C9">
+        <v>-259.76</v>
+      </c>
+      <c r="D9">
+        <v>-313.29000000000002</v>
+      </c>
+      <c r="E9">
+        <v>-393.04</v>
+      </c>
+      <c r="F9">
+        <v>-319.36</v>
+      </c>
+      <c r="G9">
+        <v>-373.86</v>
+      </c>
+      <c r="H9">
+        <v>-435.04</v>
+      </c>
+      <c r="I9">
+        <v>-472.52</v>
+      </c>
+      <c r="J9">
+        <v>-542.74</v>
+      </c>
+      <c r="K9">
+        <v>-622.55999999999995</v>
+      </c>
+      <c r="L9">
+        <v>-967.4</v>
+      </c>
+      <c r="M9">
+        <v>-1658.92</v>
+      </c>
+      <c r="N9">
+        <v>-1788.35</v>
+      </c>
+      <c r="O9">
+        <v>-1919.42</v>
+      </c>
+      <c r="P9">
+        <v>-1947.23</v>
+      </c>
+      <c r="Q9">
+        <v>-1922.15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>-143.72</v>
+      </c>
+      <c r="C10">
+        <v>-62.61</v>
+      </c>
+      <c r="D10">
+        <v>-78.73</v>
+      </c>
+      <c r="E10">
+        <v>-86.92</v>
+      </c>
+      <c r="F10">
+        <v>-367.21</v>
+      </c>
+      <c r="G10">
+        <v>-420.77</v>
+      </c>
+      <c r="H10">
+        <v>-377.73</v>
+      </c>
+      <c r="I10">
+        <v>-212.97</v>
+      </c>
+      <c r="J10">
+        <v>-339.49</v>
+      </c>
+      <c r="K10">
+        <v>-493.35</v>
+      </c>
+      <c r="L10">
+        <v>-466.17</v>
+      </c>
+      <c r="M10">
+        <v>-602.4</v>
+      </c>
+      <c r="N10">
+        <v>-680.98</v>
+      </c>
+      <c r="O10">
+        <v>-696.48</v>
+      </c>
+      <c r="P10">
+        <v>-1358.77</v>
+      </c>
+      <c r="Q10">
+        <v>-1519.34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <f>AVERAGE(B2:B10)</f>
+        <v>-309.75555555555553</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:Q11" si="0">AVERAGE(C2:C10)</f>
+        <v>-337.05</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>-345.98888888888888</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>-404.81888888888886</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>-602.5044444444444</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>-531.72222222222217</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>-518.13222222222225</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>-501.8322222222223</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>-563.12555555555548</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>-744.99111111111108</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>-920.07777777777767</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>-1166.9888888888888</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>-1304.0611111111109</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>-1385.2377777777776</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="0"/>
+        <v>-1642.5199999999998</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="0"/>
+        <v>-1765.9499999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data from raw to mem_grav
</commit_message>
<xml_diff>
--- a/pendulum/work_on_memory/memory_grav.xlsx
+++ b/pendulum/work_on_memory/memory_grav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sky/Documents/Work Info/Research Assistant/deap_experiments/pendulum/work_on_memory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AFB7C42-BDC5-1248-A905-765A4249B915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7F9EC9-B966-9C47-B0F0-CA9853EC7F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="3000" windowWidth="20320" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20320" yWindow="3580" windowWidth="20320" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9.81" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>Ind</t>
+  </si>
   <si>
     <t>sub(read(a0, a1), add(add(add(a2, a2), a2), add(a2, add(add(a2, write(a0, sin(0), add(sin(read(a0, limit(a2, protectedLog(a2), a2))), a2))), add(a2, sub(protectedDiv(abs(a2), a2), read(a0, read(a0, cos(conditional(a1, 0))))))))))</t>
   </si>
@@ -62,7 +65,31 @@
     <t>protectedDiv(sub(sub(0, write(a0, a2, conditional(conditional(a2, 0), sin(read(a0, 0))))), write(a0, protectedDiv(a1, a1), conditional(conditional(a2, 0), read(a0, 0)))), a2)</t>
   </si>
   <si>
-    <t>Ind</t>
+    <t>protectedDiv(sin(add(read(a0, a1), protectedDiv(a2, 0))), limit(a1, conditional(protectedDiv(write(a0, conditional(write(a0, 0, a1), a1), a2), a1), a2), a1))</t>
+  </si>
+  <si>
+    <t>sub(a2, add(sub(sub(sin(a2), read(a0, a2)), read(a0, a1)), protectedDiv(cos(protectedDiv(read(a0, 0), a2)), write(a0, a1, a2))))</t>
+  </si>
+  <si>
+    <t>protectedDiv(limit(sin(0), conditional(protectedDiv(sin(a2), protectedDiv(a2, a1)), read(a0, 0)), sub(conditional(0, limit(0, limit(a2, 0, a2), read(a0, 0))), abs(add(protectedDiv(cos(add(a1, protectedLog(a2))), conditional(a1, a1)), write(a0, 0, a1))))), sin(a2))</t>
+  </si>
+  <si>
+    <t>sub(protectedLog(protectedDiv(protectedLog(protectedDiv(a1, conditional(read(a0, read(a0, a1)), a2))), sub(a1, a2))), protectedDiv(conditional(read(a0, 0), write(a0, limit(add(0, write(a0, a2, cos(a2))), 0, 0), a1)), a2))</t>
+  </si>
+  <si>
+    <t>sub(add(add(write(a0, 0, limit(read(a0, conditional(0, a1)), a1, add(a2, a1))), read(a0, read(a0, a1))), read(a0, protectedDiv(abs(0), conditional(cos(abs(a1)), protectedDiv(a2, 0))))), sub(protectedLog(cos(0)), a1))</t>
+  </si>
+  <si>
+    <t>sub(read(a0, sin(0)), add(add(protectedDiv(a2, abs(read(a0, abs(protectedDiv(a2, a2))))), add(write(a0, read(a0, 0), a2), protectedDiv(a2, protectedDiv(a2, read(a0, protectedLog(0)))))), a2))</t>
+  </si>
+  <si>
+    <t>sub(sub(read(a0, sin(conditional(0, sin(a1)))), read(a0, write(a0, protectedLog(conditional(sub(a1, 0), 0)), write(a0, a2, protectedDiv(protectedLog(abs(protectedLog(cos(protectedLog(abs(a1)))))), a2))))), protectedDiv(a1, a2))</t>
+  </si>
+  <si>
+    <t>protectedDiv(sub(a2, read(a0, read(a0, a1))), protectedLog(conditional(protectedDiv(a1, cos(a2)), limit(protectedDiv(sin(sub(a2, a2)), protectedLog(limit(a1, protectedDiv(a1, a2), a2))), a1, protectedLog(write(a0, read(a0, cos(conditional(a2, read(a0, a1)))), write(a0, sin(a1), sin(sin(a2)))))))))</t>
+  </si>
+  <si>
+    <t>sub(write(a0, 0, protectedDiv(read(a0, a1), cos(limit(write(a0, cos(abs(limit(a1, abs(abs(0)), 0))), a1), sub(a2, 0), a1)))), write(a0, add(abs(cos(add(a1, a1))), sub(add(sub(sin(sub(0, a1)), 0), 0), a1)), limit(0, protectedDiv(limit(read(a0, read(a0, a2)), read(a0, sub(a2, a2)), sub(0, sub(abs(write(a0, a1, conditional(protectedDiv(a1, protectedLog(cos(a2))), a2))), a2))), a2), protectedDiv(read(a0, add(a2, a2)), protectedLog(cos(a2))))))</t>
   </si>
 </sst>
 </file>
@@ -414,17 +441,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -477,7 +504,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>-275.23</v>
@@ -530,7 +557,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>-63.71</v>
@@ -583,7 +610,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>-261.11</v>
@@ -636,7 +663,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>-122.45</v>
@@ -689,7 +716,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>-1058.8599999999999</v>
@@ -742,7 +769,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>-102.45</v>
@@ -795,7 +822,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>-506.76</v>
@@ -848,7 +875,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>-253.51</v>
@@ -901,7 +928,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>-143.72</v>
@@ -953,69 +980,480 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
       <c r="B11">
-        <f>AVERAGE(B2:B10)</f>
-        <v>-309.75555555555553</v>
+        <v>-1601.43</v>
       </c>
       <c r="C11">
-        <f t="shared" ref="C11:Q11" si="0">AVERAGE(C2:C10)</f>
-        <v>-337.05</v>
+        <v>-1762.92</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
-        <v>-345.98888888888888</v>
+        <v>-1793.76</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
-        <v>-404.81888888888886</v>
+        <v>-1806.8</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
-        <v>-602.5044444444444</v>
+        <v>-1829.62</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
-        <v>-531.72222222222217</v>
+        <v>-1783.36</v>
       </c>
       <c r="H11">
-        <f t="shared" si="0"/>
-        <v>-518.13222222222225</v>
+        <v>-1754.89</v>
       </c>
       <c r="I11">
-        <f t="shared" si="0"/>
-        <v>-501.8322222222223</v>
+        <v>-1654.82</v>
       </c>
       <c r="J11">
-        <f t="shared" si="0"/>
-        <v>-563.12555555555548</v>
+        <v>-1097.29</v>
       </c>
       <c r="K11">
-        <f t="shared" si="0"/>
-        <v>-744.99111111111108</v>
+        <v>-1537.21</v>
       </c>
       <c r="L11">
-        <f t="shared" si="0"/>
-        <v>-920.07777777777767</v>
+        <v>-1702.74</v>
       </c>
       <c r="M11">
-        <f t="shared" si="0"/>
-        <v>-1166.9888888888888</v>
+        <v>-1809.08</v>
       </c>
       <c r="N11">
-        <f t="shared" si="0"/>
-        <v>-1304.0611111111109</v>
+        <v>-1903.96</v>
       </c>
       <c r="O11">
-        <f t="shared" si="0"/>
-        <v>-1385.2377777777776</v>
+        <v>-1976.55</v>
       </c>
       <c r="P11">
-        <f t="shared" si="0"/>
-        <v>-1642.5199999999998</v>
+        <v>-2039.45</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="0"/>
-        <v>-1765.9499999999998</v>
+        <v>-2085</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>-777.3</v>
+      </c>
+      <c r="C12">
+        <v>-914.73</v>
+      </c>
+      <c r="D12">
+        <v>-822.22</v>
+      </c>
+      <c r="E12">
+        <v>-979.89</v>
+      </c>
+      <c r="F12">
+        <v>-872.65</v>
+      </c>
+      <c r="G12">
+        <v>-1091.69</v>
+      </c>
+      <c r="H12">
+        <v>-966.03</v>
+      </c>
+      <c r="I12">
+        <v>-715.85</v>
+      </c>
+      <c r="J12">
+        <v>-485.38</v>
+      </c>
+      <c r="K12">
+        <v>-1391.83</v>
+      </c>
+      <c r="L12">
+        <v>-1654.53</v>
+      </c>
+      <c r="M12">
+        <v>-1883.92</v>
+      </c>
+      <c r="N12">
+        <v>-1719.65</v>
+      </c>
+      <c r="O12">
+        <v>-1885.24</v>
+      </c>
+      <c r="P12">
+        <v>-2013.94</v>
+      </c>
+      <c r="Q12">
+        <v>-2022.45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>-84.64</v>
+      </c>
+      <c r="C13">
+        <v>-77.209999999999994</v>
+      </c>
+      <c r="D13">
+        <v>-97.52</v>
+      </c>
+      <c r="E13">
+        <v>-176.59</v>
+      </c>
+      <c r="F13">
+        <v>-534.52</v>
+      </c>
+      <c r="G13">
+        <v>-394.67</v>
+      </c>
+      <c r="H13">
+        <v>-431.43</v>
+      </c>
+      <c r="I13">
+        <v>-332.02</v>
+      </c>
+      <c r="J13">
+        <v>-472.42</v>
+      </c>
+      <c r="K13">
+        <v>-313.89999999999998</v>
+      </c>
+      <c r="L13">
+        <v>-259.23</v>
+      </c>
+      <c r="M13">
+        <v>-359.09</v>
+      </c>
+      <c r="N13">
+        <v>-1090.83</v>
+      </c>
+      <c r="O13">
+        <v>-1540.24</v>
+      </c>
+      <c r="P13">
+        <v>-1724.38</v>
+      </c>
+      <c r="Q13">
+        <v>-1686.35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>-735.9</v>
+      </c>
+      <c r="C14">
+        <v>-757.48</v>
+      </c>
+      <c r="D14">
+        <v>-806.37</v>
+      </c>
+      <c r="E14">
+        <v>-574.64</v>
+      </c>
+      <c r="F14">
+        <v>-586.11</v>
+      </c>
+      <c r="G14">
+        <v>-543.74</v>
+      </c>
+      <c r="H14">
+        <v>-490.72</v>
+      </c>
+      <c r="I14">
+        <v>-438.39</v>
+      </c>
+      <c r="J14">
+        <v>-449.81</v>
+      </c>
+      <c r="K14">
+        <v>-428.61</v>
+      </c>
+      <c r="L14">
+        <v>-769.46</v>
+      </c>
+      <c r="M14">
+        <v>-1307.49</v>
+      </c>
+      <c r="N14">
+        <v>-1717.2</v>
+      </c>
+      <c r="O14">
+        <v>-1833.18</v>
+      </c>
+      <c r="P14">
+        <v>-1922.43</v>
+      </c>
+      <c r="Q14">
+        <v>-1955.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>-1994.27</v>
+      </c>
+      <c r="C15">
+        <v>-2000.25</v>
+      </c>
+      <c r="D15">
+        <v>-1985.17</v>
+      </c>
+      <c r="E15">
+        <v>-1935.46</v>
+      </c>
+      <c r="F15">
+        <v>-1899.96</v>
+      </c>
+      <c r="G15">
+        <v>-1835.84</v>
+      </c>
+      <c r="H15">
+        <v>-1779.28</v>
+      </c>
+      <c r="I15">
+        <v>-1693.84</v>
+      </c>
+      <c r="J15">
+        <v>-1384.36</v>
+      </c>
+      <c r="K15">
+        <v>-1799.1</v>
+      </c>
+      <c r="L15">
+        <v>-1873.38</v>
+      </c>
+      <c r="M15">
+        <v>-2044.61</v>
+      </c>
+      <c r="N15">
+        <v>-2064.5100000000002</v>
+      </c>
+      <c r="O15">
+        <v>-2163.1999999999998</v>
+      </c>
+      <c r="P15">
+        <v>-2198.2399999999998</v>
+      </c>
+      <c r="Q15">
+        <v>-2222.87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>-199.75</v>
+      </c>
+      <c r="C16">
+        <v>-121.54</v>
+      </c>
+      <c r="D16">
+        <v>-221.3</v>
+      </c>
+      <c r="E16">
+        <v>-185.66</v>
+      </c>
+      <c r="F16">
+        <v>-602.98</v>
+      </c>
+      <c r="G16">
+        <v>-689.44</v>
+      </c>
+      <c r="H16">
+        <v>-679.79</v>
+      </c>
+      <c r="I16">
+        <v>-870.84</v>
+      </c>
+      <c r="J16">
+        <v>-1055.8</v>
+      </c>
+      <c r="K16">
+        <v>-1147.07</v>
+      </c>
+      <c r="L16">
+        <v>-1278.43</v>
+      </c>
+      <c r="M16">
+        <v>-1220.82</v>
+      </c>
+      <c r="N16">
+        <v>-1226.27</v>
+      </c>
+      <c r="O16">
+        <v>-1281.83</v>
+      </c>
+      <c r="P16">
+        <v>-1403.98</v>
+      </c>
+      <c r="Q16">
+        <v>-1589.37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>-649.85</v>
+      </c>
+      <c r="C17">
+        <v>-573.73</v>
+      </c>
+      <c r="D17">
+        <v>-666.32</v>
+      </c>
+      <c r="E17">
+        <v>-718.45</v>
+      </c>
+      <c r="F17">
+        <v>-610.42999999999995</v>
+      </c>
+      <c r="G17">
+        <v>-511.37</v>
+      </c>
+      <c r="H17">
+        <v>-394.75</v>
+      </c>
+      <c r="I17">
+        <v>-390.88</v>
+      </c>
+      <c r="J17">
+        <v>-215.67</v>
+      </c>
+      <c r="K17">
+        <v>-256.58</v>
+      </c>
+      <c r="L17">
+        <v>-402.68</v>
+      </c>
+      <c r="M17">
+        <v>-1338.68</v>
+      </c>
+      <c r="N17">
+        <v>-1588.12</v>
+      </c>
+      <c r="O17">
+        <v>-1705.61</v>
+      </c>
+      <c r="P17">
+        <v>-1866.84</v>
+      </c>
+      <c r="Q17">
+        <v>-1989.53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>-255.37</v>
+      </c>
+      <c r="C18">
+        <v>-208.79</v>
+      </c>
+      <c r="D18">
+        <v>-211.47</v>
+      </c>
+      <c r="E18">
+        <v>-189.68</v>
+      </c>
+      <c r="F18">
+        <v>-230.32</v>
+      </c>
+      <c r="G18">
+        <v>-223.29</v>
+      </c>
+      <c r="H18">
+        <v>-232.27</v>
+      </c>
+      <c r="I18">
+        <v>-396.58</v>
+      </c>
+      <c r="J18">
+        <v>-314.38</v>
+      </c>
+      <c r="K18">
+        <v>-392.85</v>
+      </c>
+      <c r="L18">
+        <v>-662.52</v>
+      </c>
+      <c r="M18">
+        <v>-1159.08</v>
+      </c>
+      <c r="N18">
+        <v>-1354.06</v>
+      </c>
+      <c r="O18">
+        <v>-1666.42</v>
+      </c>
+      <c r="P18">
+        <v>-1833.84</v>
+      </c>
+      <c r="Q18">
+        <v>-1925.19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>-134.61000000000001</v>
+      </c>
+      <c r="C19">
+        <v>-143.61000000000001</v>
+      </c>
+      <c r="D19">
+        <v>-129.91999999999999</v>
+      </c>
+      <c r="E19">
+        <v>-152.12</v>
+      </c>
+      <c r="F19">
+        <v>-160.94</v>
+      </c>
+      <c r="G19">
+        <v>-165.41</v>
+      </c>
+      <c r="H19">
+        <v>-178.39</v>
+      </c>
+      <c r="I19">
+        <v>-198.05</v>
+      </c>
+      <c r="J19">
+        <v>-245.34</v>
+      </c>
+      <c r="K19">
+        <v>-297.76</v>
+      </c>
+      <c r="L19">
+        <v>-397.98</v>
+      </c>
+      <c r="M19">
+        <v>-1401.08</v>
+      </c>
+      <c r="N19">
+        <v>-1545.8</v>
+      </c>
+      <c r="O19">
+        <v>-1657.87</v>
+      </c>
+      <c r="P19">
+        <v>-1744.01</v>
+      </c>
+      <c r="Q19">
+        <v>-1940.92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change to grav 10 and create excel move script
</commit_message>
<xml_diff>
--- a/pendulum/work_on_memory/memory_grav.xlsx
+++ b/pendulum/work_on_memory/memory_grav.xlsx
@@ -1,113 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sky/Documents/Work Info/Research Assistant/deap_experiments/pendulum/work_on_memory/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7F9EC9-B966-9C47-B0F0-CA9853EC7F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-20320" yWindow="3580" windowWidth="20320" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-20320" yWindow="3580" windowWidth="20320" windowHeight="14420" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="9.81" sheetId="1" r:id="rId1"/>
+    <sheet name="9.81" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>Ind</t>
-  </si>
-  <si>
-    <t>sub(read(a0, a1), add(add(add(a2, a2), a2), add(a2, add(add(a2, write(a0, sin(0), add(sin(read(a0, limit(a2, protectedLog(a2), a2))), a2))), add(a2, sub(protectedDiv(abs(a2), a2), read(a0, read(a0, cos(conditional(a1, 0))))))))))</t>
-  </si>
-  <si>
-    <t>protectedDiv(add(read(a0, read(a0, sub(sin(add(read(a0, a1), protectedDiv(0, a1))), protectedDiv(0, a2)))), a2), conditional(sin(sin(read(a0, a1))), write(a0, limit(protectedLog(read(a0, add(add(conditional(abs(sin(a1)), a1), a2), sin(sin(a2))))), abs(limit(0, read(a0, a2), 0)), conditional(protectedDiv(0, a1), protectedDiv(a1, conditional(a2, read(a0, 0))))), a2)))</t>
-  </si>
-  <si>
-    <t>sub(sub(limit(a2, read(a0, a2), protectedLog(read(a0, abs(0)))), a2), add(write(a0, protectedLog(sub(conditional(a1, a2), sin(a2))), write(a0, protectedDiv(a1, limit(0, 0, limit(write(a0, a1, write(a0, 0, a2)), a2, a2))), a2)), limit(sin(cos(sub(protectedLog(abs(a2)), a2))), sub(0, limit(a2, a1, 0)), a2)))</t>
-  </si>
-  <si>
-    <t>sub(sub(read(a0, a1), add(write(a0, abs(a2), protectedDiv(add(a2, a2), protectedLog(write(a0, sin(cos(0)), abs(a1))))), cos(read(a0, read(a0, abs(sub(a1, conditional(limit(a2, limit(0, a1, a2), a2), a1)))))))), sub(a2, protectedLog(a2)))</t>
-  </si>
-  <si>
-    <t>sub(read(a0, a2), write(a0, sub(conditional(write(a0, a1, protectedLog(conditional(a1, protectedLog(a1)))), add(abs(0), sub(abs(write(a0, a1, a1)), add(protectedDiv(a2, a2), limit(0, 0, 0))))), conditional(0, conditional(conditional(a2, abs(a1)), a1))), protectedDiv(a2, conditional(sub(a2, sin(sin(write(a0, abs(conditional(sin(a1), 0)), a2)))), a2))))</t>
-  </si>
-  <si>
-    <t>sub(sub(0, read(a0, a1)), add(protectedDiv(conditional(a2, read(a0, read(a0, a1))), a2), add(write(a0, a1, sin(a2)), a2)))</t>
-  </si>
-  <si>
-    <t>sub(protectedDiv(sub(protectedDiv(conditional(read(a0, a2), a2), a2), sin(limit(0, 0, a1))), cos(sub(write(a0, 0, a2), cos(limit(cos(sin(a2)), 0, read(a0, 0)))))), a2)</t>
-  </si>
-  <si>
-    <t>sub(sub(read(a0, 0), protectedDiv(limit(sin(a1), protectedDiv(a2, protectedDiv(read(a0, a2), a1)), protectedLog(read(a0, a2))), a2)), write(a0, a2, a2))</t>
-  </si>
-  <si>
-    <t>protectedDiv(sub(sub(0, write(a0, a2, conditional(conditional(a2, 0), sin(read(a0, 0))))), write(a0, protectedDiv(a1, a1), conditional(conditional(a2, 0), read(a0, 0)))), a2)</t>
-  </si>
-  <si>
-    <t>protectedDiv(sin(add(read(a0, a1), protectedDiv(a2, 0))), limit(a1, conditional(protectedDiv(write(a0, conditional(write(a0, 0, a1), a1), a2), a1), a2), a1))</t>
-  </si>
-  <si>
-    <t>sub(a2, add(sub(sub(sin(a2), read(a0, a2)), read(a0, a1)), protectedDiv(cos(protectedDiv(read(a0, 0), a2)), write(a0, a1, a2))))</t>
-  </si>
-  <si>
-    <t>protectedDiv(limit(sin(0), conditional(protectedDiv(sin(a2), protectedDiv(a2, a1)), read(a0, 0)), sub(conditional(0, limit(0, limit(a2, 0, a2), read(a0, 0))), abs(add(protectedDiv(cos(add(a1, protectedLog(a2))), conditional(a1, a1)), write(a0, 0, a1))))), sin(a2))</t>
-  </si>
-  <si>
-    <t>sub(protectedLog(protectedDiv(protectedLog(protectedDiv(a1, conditional(read(a0, read(a0, a1)), a2))), sub(a1, a2))), protectedDiv(conditional(read(a0, 0), write(a0, limit(add(0, write(a0, a2, cos(a2))), 0, 0), a1)), a2))</t>
-  </si>
-  <si>
-    <t>sub(add(add(write(a0, 0, limit(read(a0, conditional(0, a1)), a1, add(a2, a1))), read(a0, read(a0, a1))), read(a0, protectedDiv(abs(0), conditional(cos(abs(a1)), protectedDiv(a2, 0))))), sub(protectedLog(cos(0)), a1))</t>
-  </si>
-  <si>
-    <t>sub(read(a0, sin(0)), add(add(protectedDiv(a2, abs(read(a0, abs(protectedDiv(a2, a2))))), add(write(a0, read(a0, 0), a2), protectedDiv(a2, protectedDiv(a2, read(a0, protectedLog(0)))))), a2))</t>
-  </si>
-  <si>
-    <t>sub(sub(read(a0, sin(conditional(0, sin(a1)))), read(a0, write(a0, protectedLog(conditional(sub(a1, 0), 0)), write(a0, a2, protectedDiv(protectedLog(abs(protectedLog(cos(protectedLog(abs(a1)))))), a2))))), protectedDiv(a1, a2))</t>
-  </si>
-  <si>
-    <t>protectedDiv(sub(a2, read(a0, read(a0, a1))), protectedLog(conditional(protectedDiv(a1, cos(a2)), limit(protectedDiv(sin(sub(a2, a2)), protectedLog(limit(a1, protectedDiv(a1, a2), a2))), a1, protectedLog(write(a0, read(a0, cos(conditional(a2, read(a0, a1)))), write(a0, sin(a1), sin(sin(a2)))))))))</t>
-  </si>
-  <si>
-    <t>sub(write(a0, 0, protectedDiv(read(a0, a1), cos(limit(write(a0, cos(abs(limit(a1, abs(abs(0)), 0))), a1), sub(a2, 0), a1)))), write(a0, add(abs(cos(add(a1, a1))), sub(add(sub(sin(sub(0, a1)), 0), 0), a1)), limit(0, protectedDiv(limit(read(a0, read(a0, a2)), read(a0, sub(a2, a2)), sub(0, sub(abs(write(a0, a1, conditional(protectedDiv(a1, protectedLog(cos(a2))), a2))), a2))), a2), protectedDiv(read(a0, add(a2, a2)), protectedLog(cos(a2))))))</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -126,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -440,1020 +419,1117 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Ind</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="C1" t="n">
         <v>2</v>
       </c>
-      <c r="D1">
+      <c r="D1" t="n">
         <v>3</v>
       </c>
-      <c r="E1">
+      <c r="E1" t="n">
         <v>4</v>
       </c>
-      <c r="F1">
+      <c r="F1" t="n">
         <v>5</v>
       </c>
-      <c r="G1">
+      <c r="G1" t="n">
         <v>6</v>
       </c>
-      <c r="H1">
+      <c r="H1" t="n">
         <v>7</v>
       </c>
-      <c r="I1">
+      <c r="I1" t="n">
         <v>8</v>
       </c>
-      <c r="J1">
+      <c r="J1" t="n">
         <v>9.81</v>
       </c>
-      <c r="K1">
+      <c r="K1" t="n">
         <v>11</v>
       </c>
-      <c r="L1">
+      <c r="L1" t="n">
         <v>12</v>
       </c>
-      <c r="M1">
+      <c r="M1" t="n">
         <v>13</v>
       </c>
-      <c r="N1">
+      <c r="N1" t="n">
         <v>14</v>
       </c>
-      <c r="O1">
+      <c r="O1" t="n">
         <v>15</v>
       </c>
-      <c r="P1">
+      <c r="P1" t="n">
         <v>16</v>
       </c>
-      <c r="Q1">
+      <c r="Q1" t="n">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>sub(read(a0, a1), add(add(add(a2, a2), a2), add(a2, add(add(a2, write(a0, sin(0), add(sin(read(a0, limit(a2, protectedLog(a2), a2))), a2))), add(a2, sub(protectedDiv(abs(a2), a2), read(a0, read(a0, cos(conditional(a1, 0))))))))))</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>-275.23</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="n">
         <v>-242.91</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="n">
         <v>-134.72</v>
       </c>
-      <c r="E2">
-        <v>-150.97999999999999</v>
-      </c>
-      <c r="F2">
+      <c r="E2" t="n">
+        <v>-150.98</v>
+      </c>
+      <c r="F2" t="n">
         <v>-815.37</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="n">
         <v>-700.74</v>
       </c>
-      <c r="H2">
+      <c r="H2" t="n">
         <v>-709.36</v>
       </c>
-      <c r="I2">
-        <v>-682.57</v>
-      </c>
-      <c r="J2">
+      <c r="I2" t="n">
+        <v>-682.5700000000001</v>
+      </c>
+      <c r="J2" t="n">
         <v>-913.48</v>
       </c>
-      <c r="K2">
-        <v>-948.93</v>
-      </c>
-      <c r="L2">
-        <v>-1148.8800000000001</v>
-      </c>
-      <c r="M2">
+      <c r="K2" t="n">
+        <v>-948.9299999999999</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-1148.88</v>
+      </c>
+      <c r="M2" t="n">
         <v>-1135.3</v>
       </c>
-      <c r="N2">
+      <c r="N2" t="n">
         <v>-1295.02</v>
       </c>
-      <c r="O2">
+      <c r="O2" t="n">
         <v>-1344.59</v>
       </c>
-      <c r="P2">
+      <c r="P2" t="n">
         <v>-1539.4</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" t="n">
         <v>-1694.02</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>protectedDiv(add(read(a0, read(a0, sub(sin(add(read(a0, a1), protectedDiv(0, a1))), protectedDiv(0, a2)))), a2), conditional(sin(sin(read(a0, a1))), write(a0, limit(protectedLog(read(a0, add(add(conditional(abs(sin(a1)), a1), a2), sin(sin(a2))))), abs(limit(0, read(a0, a2), 0)), conditional(protectedDiv(0, a1), protectedDiv(a1, conditional(a2, read(a0, 0))))), a2)))</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>-63.71</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="n">
         <v>-79.34</v>
       </c>
-      <c r="D3">
-        <v>-71.709999999999994</v>
-      </c>
-      <c r="E3">
+      <c r="D3" t="n">
+        <v>-71.70999999999999</v>
+      </c>
+      <c r="E3" t="n">
         <v>-107.46</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="n">
         <v>-662.35</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="n">
         <v>-360.37</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="n">
         <v>-363.8</v>
       </c>
-      <c r="I3">
+      <c r="I3" t="n">
         <v>-338.91</v>
       </c>
-      <c r="J3">
+      <c r="J3" t="n">
         <v>-351.74</v>
       </c>
-      <c r="K3">
+      <c r="K3" t="n">
         <v>-740.29</v>
       </c>
-      <c r="L3">
+      <c r="L3" t="n">
         <v>-729.01</v>
       </c>
-      <c r="M3">
+      <c r="M3" t="n">
         <v>-964.33</v>
       </c>
-      <c r="N3">
+      <c r="N3" t="n">
         <v>-826.55</v>
       </c>
-      <c r="O3">
-        <v>-1287.4100000000001</v>
-      </c>
-      <c r="P3">
+      <c r="O3" t="n">
+        <v>-1287.41</v>
+      </c>
+      <c r="P3" t="n">
         <v>-1439.09</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" t="n">
         <v>-1654.47</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>sub(sub(limit(a2, read(a0, a2), protectedLog(read(a0, abs(0)))), a2), add(write(a0, protectedLog(sub(conditional(a1, a2), sin(a2))), write(a0, protectedDiv(a1, limit(0, 0, limit(write(a0, a1, write(a0, 0, a2)), a2, a2))), a2)), limit(sin(cos(sub(protectedLog(abs(a2)), a2))), sub(0, limit(a2, a1, 0)), a2)))</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>-261.11</v>
       </c>
-      <c r="C4">
-        <v>-259.39999999999998</v>
-      </c>
-      <c r="D4">
+      <c r="C4" t="n">
+        <v>-259.4</v>
+      </c>
+      <c r="D4" t="n">
         <v>-232.87</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="n">
         <v>-482.79</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="n">
         <v>-496.35</v>
       </c>
-      <c r="G4">
+      <c r="G4" t="n">
         <v>-447.32</v>
       </c>
-      <c r="H4">
+      <c r="H4" t="n">
         <v>-482.08</v>
       </c>
-      <c r="I4">
+      <c r="I4" t="n">
         <v>-662.74</v>
       </c>
-      <c r="J4">
+      <c r="J4" t="n">
         <v>-831.64</v>
       </c>
-      <c r="K4">
+      <c r="K4" t="n">
         <v>-965.16</v>
       </c>
-      <c r="L4">
+      <c r="L4" t="n">
         <v>-1043.54</v>
       </c>
-      <c r="M4">
+      <c r="M4" t="n">
         <v>-1173.49</v>
       </c>
-      <c r="N4">
+      <c r="N4" t="n">
         <v>-1281.57</v>
       </c>
-      <c r="O4">
-        <v>-1170.3699999999999</v>
-      </c>
-      <c r="P4">
+      <c r="O4" t="n">
+        <v>-1170.37</v>
+      </c>
+      <c r="P4" t="n">
         <v>-1585.31</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" t="n">
         <v>-1700.21</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>sub(sub(read(a0, a1), add(write(a0, abs(a2), protectedDiv(add(a2, a2), protectedLog(write(a0, sin(cos(0)), abs(a1))))), cos(read(a0, read(a0, abs(sub(a1, conditional(limit(a2, limit(0, a1, a2), a2), a1)))))))), sub(a2, protectedLog(a2)))</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>-122.45</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="n">
         <v>-188.19</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="n">
         <v>-313.43</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="n">
         <v>-320.75</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="n">
         <v>-442.52</v>
       </c>
-      <c r="G5">
+      <c r="G5" t="n">
         <v>-421.35</v>
       </c>
-      <c r="H5">
+      <c r="H5" t="n">
         <v>-356.11</v>
       </c>
-      <c r="I5">
+      <c r="I5" t="n">
         <v>-345.63</v>
       </c>
-      <c r="J5">
+      <c r="J5" t="n">
         <v>-303.81</v>
       </c>
-      <c r="K5">
+      <c r="K5" t="n">
         <v>-322.44</v>
       </c>
-      <c r="L5">
+      <c r="L5" t="n">
         <v>-440.37</v>
       </c>
-      <c r="M5">
-        <v>-1043.8900000000001</v>
-      </c>
-      <c r="N5">
+      <c r="M5" t="n">
+        <v>-1043.89</v>
+      </c>
+      <c r="N5" t="n">
         <v>-1538.81</v>
       </c>
-      <c r="O5">
+      <c r="O5" t="n">
         <v>-1513.8</v>
       </c>
-      <c r="P5">
+      <c r="P5" t="n">
         <v>-1678.98</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" t="n">
         <v>-1853.78</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>-1058.8599999999999</v>
-      </c>
-      <c r="C6">
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>sub(read(a0, a2), write(a0, sub(conditional(write(a0, a1, protectedLog(conditional(a1, protectedLog(a1)))), add(abs(0), sub(abs(write(a0, a1, a1)), add(protectedDiv(a2, a2), limit(0, 0, 0))))), conditional(0, conditional(conditional(a2, abs(a1)), a1))), protectedDiv(a2, conditional(sub(a2, sin(sin(write(a0, abs(conditional(sin(a1), 0)), a2)))), a2))))</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-1058.86</v>
+      </c>
+      <c r="C6" t="n">
         <v>-1048.5</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="n">
         <v>-1014.58</v>
       </c>
-      <c r="E6">
+      <c r="E6" t="n">
         <v>-1044.93</v>
       </c>
-      <c r="F6">
+      <c r="F6" t="n">
         <v>-1054.05</v>
       </c>
-      <c r="G6">
+      <c r="G6" t="n">
         <v>-1071.25</v>
       </c>
-      <c r="H6">
+      <c r="H6" t="n">
         <v>-952.87</v>
       </c>
-      <c r="I6">
+      <c r="I6" t="n">
         <v>-742.33</v>
       </c>
-      <c r="J6">
+      <c r="J6" t="n">
         <v>-612.87</v>
       </c>
-      <c r="K6">
+      <c r="K6" t="n">
         <v>-1153.49</v>
       </c>
-      <c r="L6">
+      <c r="L6" t="n">
         <v>-1467.79</v>
       </c>
-      <c r="M6">
+      <c r="M6" t="n">
         <v>-1598.73</v>
       </c>
-      <c r="N6">
+      <c r="N6" t="n">
         <v>-1752.86</v>
       </c>
-      <c r="O6">
+      <c r="O6" t="n">
         <v>-1846.33</v>
       </c>
-      <c r="P6">
+      <c r="P6" t="n">
         <v>-1944.15</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" t="n">
         <v>-2005.55</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>sub(sub(0, read(a0, a1)), add(protectedDiv(conditional(a2, read(a0, read(a0, a1))), a2), add(write(a0, a1, sin(a2)), a2)))</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>-102.45</v>
       </c>
-      <c r="C7">
-        <v>-79.069999999999993</v>
-      </c>
-      <c r="D7">
+      <c r="C7" t="n">
+        <v>-79.06999999999999</v>
+      </c>
+      <c r="D7" t="n">
         <v>-74.41</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="n">
         <v>-117.78</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="n">
         <v>-501.02</v>
       </c>
-      <c r="G7">
-        <v>-306.77999999999997</v>
-      </c>
-      <c r="H7">
+      <c r="G7" t="n">
+        <v>-306.78</v>
+      </c>
+      <c r="H7" t="n">
         <v>-426.89</v>
       </c>
-      <c r="I7">
-        <v>-289.20999999999998</v>
-      </c>
-      <c r="J7">
-        <v>-327.29000000000002</v>
-      </c>
-      <c r="K7">
-        <v>-568.05999999999995</v>
-      </c>
-      <c r="L7">
+      <c r="I7" t="n">
+        <v>-289.21</v>
+      </c>
+      <c r="J7" t="n">
+        <v>-327.29</v>
+      </c>
+      <c r="K7" t="n">
+        <v>-568.0599999999999</v>
+      </c>
+      <c r="L7" t="n">
         <v>-650.11</v>
       </c>
-      <c r="M7">
+      <c r="M7" t="n">
         <v>-758.64</v>
       </c>
-      <c r="N7">
+      <c r="N7" t="n">
         <v>-882.11</v>
       </c>
-      <c r="O7">
+      <c r="O7" t="n">
         <v>-915.95</v>
       </c>
-      <c r="P7">
+      <c r="P7" t="n">
         <v>-1393.81</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" t="n">
         <v>-1571.79</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>sub(protectedDiv(sub(protectedDiv(conditional(read(a0, a2), a2), a2), sin(limit(0, 0, a1))), cos(sub(write(a0, 0, a2), cos(limit(cos(sin(a2)), 0, read(a0, 0)))))), a2)</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>-506.76</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="n">
         <v>-813.67</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="n">
         <v>-880.16</v>
       </c>
-      <c r="E8">
+      <c r="E8" t="n">
         <v>-938.72</v>
       </c>
-      <c r="F8">
-        <v>-764.31</v>
-      </c>
-      <c r="G8">
-        <v>-683.06</v>
-      </c>
-      <c r="H8">
-        <v>-559.30999999999995</v>
-      </c>
-      <c r="I8">
+      <c r="F8" t="n">
+        <v>-764.3099999999999</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-683.0599999999999</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-559.3099999999999</v>
+      </c>
+      <c r="I8" t="n">
         <v>-769.61</v>
       </c>
-      <c r="J8">
-        <v>-845.07</v>
-      </c>
-      <c r="K8">
+      <c r="J8" t="n">
+        <v>-845.0700000000001</v>
+      </c>
+      <c r="K8" t="n">
         <v>-890.64</v>
       </c>
-      <c r="L8">
+      <c r="L8" t="n">
         <v>-1367.43</v>
       </c>
-      <c r="M8">
+      <c r="M8" t="n">
         <v>-1567.2</v>
       </c>
-      <c r="N8">
+      <c r="N8" t="n">
         <v>-1690.3</v>
       </c>
-      <c r="O8">
+      <c r="O8" t="n">
         <v>-1772.79</v>
       </c>
-      <c r="P8">
+      <c r="P8" t="n">
         <v>-1895.94</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" t="n">
         <v>-1972.24</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>sub(sub(read(a0, 0), protectedDiv(limit(sin(a1), protectedDiv(a2, protectedDiv(read(a0, a2), a1)), protectedLog(read(a0, a2))), a2)), write(a0, a2, a2))</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
         <v>-253.51</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="n">
         <v>-259.76</v>
       </c>
-      <c r="D9">
-        <v>-313.29000000000002</v>
-      </c>
-      <c r="E9">
+      <c r="D9" t="n">
+        <v>-313.29</v>
+      </c>
+      <c r="E9" t="n">
         <v>-393.04</v>
       </c>
-      <c r="F9">
+      <c r="F9" t="n">
         <v>-319.36</v>
       </c>
-      <c r="G9">
+      <c r="G9" t="n">
         <v>-373.86</v>
       </c>
-      <c r="H9">
+      <c r="H9" t="n">
         <v>-435.04</v>
       </c>
-      <c r="I9">
+      <c r="I9" t="n">
         <v>-472.52</v>
       </c>
-      <c r="J9">
+      <c r="J9" t="n">
         <v>-542.74</v>
       </c>
-      <c r="K9">
-        <v>-622.55999999999995</v>
-      </c>
-      <c r="L9">
+      <c r="K9" t="n">
+        <v>-622.5599999999999</v>
+      </c>
+      <c r="L9" t="n">
         <v>-967.4</v>
       </c>
-      <c r="M9">
+      <c r="M9" t="n">
         <v>-1658.92</v>
       </c>
-      <c r="N9">
+      <c r="N9" t="n">
         <v>-1788.35</v>
       </c>
-      <c r="O9">
+      <c r="O9" t="n">
         <v>-1919.42</v>
       </c>
-      <c r="P9">
+      <c r="P9" t="n">
         <v>-1947.23</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" t="n">
         <v>-1922.15</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>protectedDiv(sub(sub(0, write(a0, a2, conditional(conditional(a2, 0), sin(read(a0, 0))))), write(a0, protectedDiv(a1, a1), conditional(conditional(a2, 0), read(a0, 0)))), a2)</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
         <v>-143.72</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="n">
         <v>-62.61</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="n">
         <v>-78.73</v>
       </c>
-      <c r="E10">
+      <c r="E10" t="n">
         <v>-86.92</v>
       </c>
-      <c r="F10">
+      <c r="F10" t="n">
         <v>-367.21</v>
       </c>
-      <c r="G10">
+      <c r="G10" t="n">
         <v>-420.77</v>
       </c>
-      <c r="H10">
+      <c r="H10" t="n">
         <v>-377.73</v>
       </c>
-      <c r="I10">
+      <c r="I10" t="n">
         <v>-212.97</v>
       </c>
-      <c r="J10">
+      <c r="J10" t="n">
         <v>-339.49</v>
       </c>
-      <c r="K10">
+      <c r="K10" t="n">
         <v>-493.35</v>
       </c>
-      <c r="L10">
+      <c r="L10" t="n">
         <v>-466.17</v>
       </c>
-      <c r="M10">
+      <c r="M10" t="n">
         <v>-602.4</v>
       </c>
-      <c r="N10">
+      <c r="N10" t="n">
         <v>-680.98</v>
       </c>
-      <c r="O10">
+      <c r="O10" t="n">
         <v>-696.48</v>
       </c>
-      <c r="P10">
+      <c r="P10" t="n">
         <v>-1358.77</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" t="n">
         <v>-1519.34</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11">
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>protectedDiv(sin(add(read(a0, a1), protectedDiv(a2, 0))), limit(a1, conditional(protectedDiv(write(a0, conditional(write(a0, 0, a1), a1), a2), a1), a2), a1))</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
         <v>-1601.43</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="n">
         <v>-1762.92</v>
       </c>
-      <c r="D11">
+      <c r="D11" t="n">
         <v>-1793.76</v>
       </c>
-      <c r="E11">
+      <c r="E11" t="n">
         <v>-1806.8</v>
       </c>
-      <c r="F11">
+      <c r="F11" t="n">
         <v>-1829.62</v>
       </c>
-      <c r="G11">
+      <c r="G11" t="n">
         <v>-1783.36</v>
       </c>
-      <c r="H11">
+      <c r="H11" t="n">
         <v>-1754.89</v>
       </c>
-      <c r="I11">
+      <c r="I11" t="n">
         <v>-1654.82</v>
       </c>
-      <c r="J11">
+      <c r="J11" t="n">
         <v>-1097.29</v>
       </c>
-      <c r="K11">
+      <c r="K11" t="n">
         <v>-1537.21</v>
       </c>
-      <c r="L11">
+      <c r="L11" t="n">
         <v>-1702.74</v>
       </c>
-      <c r="M11">
+      <c r="M11" t="n">
         <v>-1809.08</v>
       </c>
-      <c r="N11">
+      <c r="N11" t="n">
         <v>-1903.96</v>
       </c>
-      <c r="O11">
+      <c r="O11" t="n">
         <v>-1976.55</v>
       </c>
-      <c r="P11">
+      <c r="P11" t="n">
         <v>-2039.45</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" t="n">
         <v>-2085</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>sub(a2, add(sub(sub(sin(a2), read(a0, a2)), read(a0, a1)), protectedDiv(cos(protectedDiv(read(a0, 0), a2)), write(a0, a1, a2))))</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
         <v>-777.3</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="n">
         <v>-914.73</v>
       </c>
-      <c r="D12">
+      <c r="D12" t="n">
         <v>-822.22</v>
       </c>
-      <c r="E12">
+      <c r="E12" t="n">
         <v>-979.89</v>
       </c>
-      <c r="F12">
+      <c r="F12" t="n">
         <v>-872.65</v>
       </c>
-      <c r="G12">
+      <c r="G12" t="n">
         <v>-1091.69</v>
       </c>
-      <c r="H12">
+      <c r="H12" t="n">
         <v>-966.03</v>
       </c>
-      <c r="I12">
+      <c r="I12" t="n">
         <v>-715.85</v>
       </c>
-      <c r="J12">
+      <c r="J12" t="n">
         <v>-485.38</v>
       </c>
-      <c r="K12">
+      <c r="K12" t="n">
         <v>-1391.83</v>
       </c>
-      <c r="L12">
+      <c r="L12" t="n">
         <v>-1654.53</v>
       </c>
-      <c r="M12">
+      <c r="M12" t="n">
         <v>-1883.92</v>
       </c>
-      <c r="N12">
+      <c r="N12" t="n">
         <v>-1719.65</v>
       </c>
-      <c r="O12">
+      <c r="O12" t="n">
         <v>-1885.24</v>
       </c>
-      <c r="P12">
+      <c r="P12" t="n">
         <v>-2013.94</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" t="n">
         <v>-2022.45</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>protectedDiv(limit(sin(0), conditional(protectedDiv(sin(a2), protectedDiv(a2, a1)), read(a0, 0)), sub(conditional(0, limit(0, limit(a2, 0, a2), read(a0, 0))), abs(add(protectedDiv(cos(add(a1, protectedLog(a2))), conditional(a1, a1)), write(a0, 0, a1))))), sin(a2))</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
         <v>-84.64</v>
       </c>
-      <c r="C13">
-        <v>-77.209999999999994</v>
-      </c>
-      <c r="D13">
+      <c r="C13" t="n">
+        <v>-77.20999999999999</v>
+      </c>
+      <c r="D13" t="n">
         <v>-97.52</v>
       </c>
-      <c r="E13">
+      <c r="E13" t="n">
         <v>-176.59</v>
       </c>
-      <c r="F13">
+      <c r="F13" t="n">
         <v>-534.52</v>
       </c>
-      <c r="G13">
+      <c r="G13" t="n">
         <v>-394.67</v>
       </c>
-      <c r="H13">
+      <c r="H13" t="n">
         <v>-431.43</v>
       </c>
-      <c r="I13">
+      <c r="I13" t="n">
         <v>-332.02</v>
       </c>
-      <c r="J13">
+      <c r="J13" t="n">
         <v>-472.42</v>
       </c>
-      <c r="K13">
-        <v>-313.89999999999998</v>
-      </c>
-      <c r="L13">
+      <c r="K13" t="n">
+        <v>-313.9</v>
+      </c>
+      <c r="L13" t="n">
         <v>-259.23</v>
       </c>
-      <c r="M13">
+      <c r="M13" t="n">
         <v>-359.09</v>
       </c>
-      <c r="N13">
+      <c r="N13" t="n">
         <v>-1090.83</v>
       </c>
-      <c r="O13">
+      <c r="O13" t="n">
         <v>-1540.24</v>
       </c>
-      <c r="P13">
+      <c r="P13" t="n">
         <v>-1724.38</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" t="n">
         <v>-1686.35</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>sub(protectedLog(protectedDiv(protectedLog(protectedDiv(a1, conditional(read(a0, read(a0, a1)), a2))), sub(a1, a2))), protectedDiv(conditional(read(a0, 0), write(a0, limit(add(0, write(a0, a2, cos(a2))), 0, 0), a1)), a2))</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
         <v>-735.9</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="n">
         <v>-757.48</v>
       </c>
-      <c r="D14">
+      <c r="D14" t="n">
         <v>-806.37</v>
       </c>
-      <c r="E14">
+      <c r="E14" t="n">
         <v>-574.64</v>
       </c>
-      <c r="F14">
+      <c r="F14" t="n">
         <v>-586.11</v>
       </c>
-      <c r="G14">
+      <c r="G14" t="n">
         <v>-543.74</v>
       </c>
-      <c r="H14">
+      <c r="H14" t="n">
         <v>-490.72</v>
       </c>
-      <c r="I14">
+      <c r="I14" t="n">
         <v>-438.39</v>
       </c>
-      <c r="J14">
+      <c r="J14" t="n">
         <v>-449.81</v>
       </c>
-      <c r="K14">
+      <c r="K14" t="n">
         <v>-428.61</v>
       </c>
-      <c r="L14">
+      <c r="L14" t="n">
         <v>-769.46</v>
       </c>
-      <c r="M14">
+      <c r="M14" t="n">
         <v>-1307.49</v>
       </c>
-      <c r="N14">
+      <c r="N14" t="n">
         <v>-1717.2</v>
       </c>
-      <c r="O14">
+      <c r="O14" t="n">
         <v>-1833.18</v>
       </c>
-      <c r="P14">
+      <c r="P14" t="n">
         <v>-1922.43</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" t="n">
         <v>-1955.6</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15">
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>sub(add(add(write(a0, 0, limit(read(a0, conditional(0, a1)), a1, add(a2, a1))), read(a0, read(a0, a1))), read(a0, protectedDiv(abs(0), conditional(cos(abs(a1)), protectedDiv(a2, 0))))), sub(protectedLog(cos(0)), a1))</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
         <v>-1994.27</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="n">
         <v>-2000.25</v>
       </c>
-      <c r="D15">
+      <c r="D15" t="n">
         <v>-1985.17</v>
       </c>
-      <c r="E15">
+      <c r="E15" t="n">
         <v>-1935.46</v>
       </c>
-      <c r="F15">
+      <c r="F15" t="n">
         <v>-1899.96</v>
       </c>
-      <c r="G15">
+      <c r="G15" t="n">
         <v>-1835.84</v>
       </c>
-      <c r="H15">
+      <c r="H15" t="n">
         <v>-1779.28</v>
       </c>
-      <c r="I15">
+      <c r="I15" t="n">
         <v>-1693.84</v>
       </c>
-      <c r="J15">
+      <c r="J15" t="n">
         <v>-1384.36</v>
       </c>
-      <c r="K15">
+      <c r="K15" t="n">
         <v>-1799.1</v>
       </c>
-      <c r="L15">
+      <c r="L15" t="n">
         <v>-1873.38</v>
       </c>
-      <c r="M15">
+      <c r="M15" t="n">
         <v>-2044.61</v>
       </c>
-      <c r="N15">
-        <v>-2064.5100000000002</v>
-      </c>
-      <c r="O15">
-        <v>-2163.1999999999998</v>
-      </c>
-      <c r="P15">
-        <v>-2198.2399999999998</v>
-      </c>
-      <c r="Q15">
+      <c r="N15" t="n">
+        <v>-2064.51</v>
+      </c>
+      <c r="O15" t="n">
+        <v>-2163.2</v>
+      </c>
+      <c r="P15" t="n">
+        <v>-2198.24</v>
+      </c>
+      <c r="Q15" t="n">
         <v>-2222.87</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16">
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>sub(read(a0, sin(0)), add(add(protectedDiv(a2, abs(read(a0, abs(protectedDiv(a2, a2))))), add(write(a0, read(a0, 0), a2), protectedDiv(a2, protectedDiv(a2, read(a0, protectedLog(0)))))), a2))</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
         <v>-199.75</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="n">
         <v>-121.54</v>
       </c>
-      <c r="D16">
+      <c r="D16" t="n">
         <v>-221.3</v>
       </c>
-      <c r="E16">
+      <c r="E16" t="n">
         <v>-185.66</v>
       </c>
-      <c r="F16">
+      <c r="F16" t="n">
         <v>-602.98</v>
       </c>
-      <c r="G16">
-        <v>-689.44</v>
-      </c>
-      <c r="H16">
+      <c r="G16" t="n">
+        <v>-689.4400000000001</v>
+      </c>
+      <c r="H16" t="n">
         <v>-679.79</v>
       </c>
-      <c r="I16">
+      <c r="I16" t="n">
         <v>-870.84</v>
       </c>
-      <c r="J16">
+      <c r="J16" t="n">
         <v>-1055.8</v>
       </c>
-      <c r="K16">
+      <c r="K16" t="n">
         <v>-1147.07</v>
       </c>
-      <c r="L16">
+      <c r="L16" t="n">
         <v>-1278.43</v>
       </c>
-      <c r="M16">
+      <c r="M16" t="n">
         <v>-1220.82</v>
       </c>
-      <c r="N16">
+      <c r="N16" t="n">
         <v>-1226.27</v>
       </c>
-      <c r="O16">
+      <c r="O16" t="n">
         <v>-1281.83</v>
       </c>
-      <c r="P16">
+      <c r="P16" t="n">
         <v>-1403.98</v>
       </c>
-      <c r="Q16">
+      <c r="Q16" t="n">
         <v>-1589.37</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17">
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>sub(sub(read(a0, sin(conditional(0, sin(a1)))), read(a0, write(a0, protectedLog(conditional(sub(a1, 0), 0)), write(a0, a2, protectedDiv(protectedLog(abs(protectedLog(cos(protectedLog(abs(a1)))))), a2))))), protectedDiv(a1, a2))</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
         <v>-649.85</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="n">
         <v>-573.73</v>
       </c>
-      <c r="D17">
-        <v>-666.32</v>
-      </c>
-      <c r="E17">
+      <c r="D17" t="n">
+        <v>-666.3200000000001</v>
+      </c>
+      <c r="E17" t="n">
         <v>-718.45</v>
       </c>
-      <c r="F17">
-        <v>-610.42999999999995</v>
-      </c>
-      <c r="G17">
+      <c r="F17" t="n">
+        <v>-610.4299999999999</v>
+      </c>
+      <c r="G17" t="n">
         <v>-511.37</v>
       </c>
-      <c r="H17">
+      <c r="H17" t="n">
         <v>-394.75</v>
       </c>
-      <c r="I17">
+      <c r="I17" t="n">
         <v>-390.88</v>
       </c>
-      <c r="J17">
+      <c r="J17" t="n">
         <v>-215.67</v>
       </c>
-      <c r="K17">
+      <c r="K17" t="n">
         <v>-256.58</v>
       </c>
-      <c r="L17">
+      <c r="L17" t="n">
         <v>-402.68</v>
       </c>
-      <c r="M17">
+      <c r="M17" t="n">
         <v>-1338.68</v>
       </c>
-      <c r="N17">
+      <c r="N17" t="n">
         <v>-1588.12</v>
       </c>
-      <c r="O17">
+      <c r="O17" t="n">
         <v>-1705.61</v>
       </c>
-      <c r="P17">
+      <c r="P17" t="n">
         <v>-1866.84</v>
       </c>
-      <c r="Q17">
+      <c r="Q17" t="n">
         <v>-1989.53</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18">
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>protectedDiv(sub(a2, read(a0, read(a0, a1))), protectedLog(conditional(protectedDiv(a1, cos(a2)), limit(protectedDiv(sin(sub(a2, a2)), protectedLog(limit(a1, protectedDiv(a1, a2), a2))), a1, protectedLog(write(a0, read(a0, cos(conditional(a2, read(a0, a1)))), write(a0, sin(a1), sin(sin(a2)))))))))</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
         <v>-255.37</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="n">
         <v>-208.79</v>
       </c>
-      <c r="D18">
+      <c r="D18" t="n">
         <v>-211.47</v>
       </c>
-      <c r="E18">
+      <c r="E18" t="n">
         <v>-189.68</v>
       </c>
-      <c r="F18">
+      <c r="F18" t="n">
         <v>-230.32</v>
       </c>
-      <c r="G18">
+      <c r="G18" t="n">
         <v>-223.29</v>
       </c>
-      <c r="H18">
+      <c r="H18" t="n">
         <v>-232.27</v>
       </c>
-      <c r="I18">
+      <c r="I18" t="n">
         <v>-396.58</v>
       </c>
-      <c r="J18">
+      <c r="J18" t="n">
         <v>-314.38</v>
       </c>
-      <c r="K18">
+      <c r="K18" t="n">
         <v>-392.85</v>
       </c>
-      <c r="L18">
+      <c r="L18" t="n">
         <v>-662.52</v>
       </c>
-      <c r="M18">
+      <c r="M18" t="n">
         <v>-1159.08</v>
       </c>
-      <c r="N18">
+      <c r="N18" t="n">
         <v>-1354.06</v>
       </c>
-      <c r="O18">
+      <c r="O18" t="n">
         <v>-1666.42</v>
       </c>
-      <c r="P18">
+      <c r="P18" t="n">
         <v>-1833.84</v>
       </c>
-      <c r="Q18">
+      <c r="Q18" t="n">
         <v>-1925.19</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>-134.61000000000001</v>
-      </c>
-      <c r="C19">
-        <v>-143.61000000000001</v>
-      </c>
-      <c r="D19">
-        <v>-129.91999999999999</v>
-      </c>
-      <c r="E19">
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>sub(write(a0, 0, protectedDiv(read(a0, a1), cos(limit(write(a0, cos(abs(limit(a1, abs(abs(0)), 0))), a1), sub(a2, 0), a1)))), write(a0, add(abs(cos(add(a1, a1))), sub(add(sub(sin(sub(0, a1)), 0), 0), a1)), limit(0, protectedDiv(limit(read(a0, read(a0, a2)), read(a0, sub(a2, a2)), sub(0, sub(abs(write(a0, a1, conditional(protectedDiv(a1, protectedLog(cos(a2))), a2))), a2))), a2), protectedDiv(read(a0, add(a2, a2)), protectedLog(cos(a2))))))</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>-134.61</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-143.61</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-129.92</v>
+      </c>
+      <c r="E19" t="n">
         <v>-152.12</v>
       </c>
-      <c r="F19">
+      <c r="F19" t="n">
         <v>-160.94</v>
       </c>
-      <c r="G19">
+      <c r="G19" t="n">
         <v>-165.41</v>
       </c>
-      <c r="H19">
+      <c r="H19" t="n">
         <v>-178.39</v>
       </c>
-      <c r="I19">
+      <c r="I19" t="n">
         <v>-198.05</v>
       </c>
-      <c r="J19">
+      <c r="J19" t="n">
         <v>-245.34</v>
       </c>
-      <c r="K19">
+      <c r="K19" t="n">
         <v>-297.76</v>
       </c>
-      <c r="L19">
+      <c r="L19" t="n">
         <v>-397.98</v>
       </c>
-      <c r="M19">
+      <c r="M19" t="n">
         <v>-1401.08</v>
       </c>
-      <c r="N19">
+      <c r="N19" t="n">
         <v>-1545.8</v>
       </c>
-      <c r="O19">
+      <c r="O19" t="n">
         <v>-1657.87</v>
       </c>
-      <c r="P19">
+      <c r="P19" t="n">
         <v>-1744.01</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" t="n">
         <v>-1940.92</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>sub(sub(sub(protectedDiv(cos(a1), a2), protectedDiv(protectedDiv(abs(a2), read(a0, a1)), abs(read(a0, cos(a1))))), write(a0, a1, write(a0, limit(limit(protectedDiv(cos(write(a0, 0, a1)), a2), protectedLog(a1), a1), protectedLog(a2), a1), a2))), protectedLog(0))</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>-109.73</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-154.09</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-521.14</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-522.01</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-535.98</v>
+      </c>
+      <c r="G20" t="n">
+        <v>-497.87</v>
+      </c>
+      <c r="H20" t="n">
+        <v>-513.01</v>
+      </c>
+      <c r="I20" t="n">
+        <v>-448.24</v>
+      </c>
+      <c r="J20" t="n">
+        <v>-461.42</v>
+      </c>
+      <c r="K20" t="n">
+        <v>-487.28</v>
+      </c>
+      <c r="L20" t="n">
+        <v>-582.3099999999999</v>
+      </c>
+      <c r="M20" t="n">
+        <v>-623.05</v>
+      </c>
+      <c r="N20" t="n">
+        <v>-1488.05</v>
+      </c>
+      <c r="O20" t="n">
+        <v>-1664.75</v>
+      </c>
+      <c r="P20" t="n">
+        <v>-1765.01</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>-1887.79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prepare full obs for testing
</commit_message>
<xml_diff>
--- a/pendulum/work_on_memory/memory_grav.xlsx
+++ b/pendulum/work_on_memory/memory_grav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sky/Documents/Work Info/Research Assistant/deap_experiments/pendulum/work_on_memory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BCDEB5-7D53-CA4C-908B-754181E460E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6267F6-B34A-8141-B357-BA40032E14ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9.81" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>Ind</t>
   </si>
@@ -95,9 +95,6 @@
   <si>
     <t>sub(sub(sub(protectedDiv(cos(a1), a2), protectedDiv(protectedDiv(abs(a2), read(a0, a1)), abs(read(a0, cos(a1))))), write(a0, a1, write(a0, limit(limit(protectedDiv(cos(write(a0, 0, a1)), a2), protectedLog(a1), a1), protectedLog(a2), a1), a2))), protectedLog(0))</t>
   </si>
-  <si>
-    <t>Removed outliers</t>
-  </si>
 </sst>
 </file>
 
@@ -149,6 +146,1793 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'9.81'!$B$20:$Q$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>-459.54388888888883</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-483.29444444444459</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-519.69500000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-546.65222222222246</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-679.55555555555543</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-636.16277777777805</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-618.38222222222214</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-606.31499999999994</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-590.9516666666666</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-755.75666666666677</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-910.89833333333343</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1225.0594444444446</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-1426.7855555555552</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1555.3166666666664</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1741.7027777777776</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-1844.0594444444441</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F4AE-2E43-8407-0D8BC6861E12}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1205581168"/>
+        <c:axId val="1205572544"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1205581168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1205572544"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1205572544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1205581168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'9.81'!$B$39:$Q$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>-292.25562499999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-308.50812499999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-348.47375000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-381.09250000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-531.40125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-489.48312500000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-474.79437500000006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-472.81312500000007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-509.71750000000009</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-641.70687500000008</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-801.25312500000007</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1137.3362500000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-1357.1043749999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1490.996875</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1694.5599999999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-1805.3249999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2600-234F-82E0-FD6C6A8229A6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1048293440"/>
+        <c:axId val="1047827264"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1048293440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1047827264"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1047827264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1048293440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>374650</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BF6936C-E337-C17A-3333-A45E4EE671B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>641350</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>180340</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3F1D83F-1F4D-3E77-0F75-4B642A6E24BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -448,15 +2232,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S19"/>
+  <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="U48" sqref="U48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -508,11 +2292,8 @@
       <c r="Q1">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -565,7 +2346,7 @@
         <v>-1694.02</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -618,7 +2399,7 @@
         <v>-1654.47</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -671,7 +2452,7 @@
         <v>-1700.21</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -724,7 +2505,7 @@
         <v>-1853.78</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -777,7 +2558,7 @@
         <v>-1571.79</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -830,7 +2611,7 @@
         <v>-1972.24</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -883,7 +2664,7 @@
         <v>-1922.15</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -936,7 +2717,7 @@
         <v>-1519.34</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -989,7 +2770,7 @@
         <v>-2085</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1042,7 +2823,7 @@
         <v>-2022.45</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1095,7 +2876,7 @@
         <v>-1686.35</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1148,7 +2929,7 @@
         <v>-1955.6</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1201,7 +2982,7 @@
         <v>-2222.87</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1254,7 +3035,7 @@
         <v>-1589.37</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1466,9 +3247,1043 @@
         <v>-1887.79</v>
       </c>
     </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <f>AVERAGE(B2:B19)</f>
+        <v>-459.54388888888883</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ref="C20:Q20" si="0">AVERAGE(C2:C19)</f>
+        <v>-483.29444444444459</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>-519.69500000000005</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>-546.65222222222246</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>-679.55555555555543</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>-636.16277777777805</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>-618.38222222222214</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>-606.31499999999994</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>-590.9516666666666</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="0"/>
+        <v>-755.75666666666677</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>-910.89833333333343</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="0"/>
+        <v>-1225.0594444444446</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="0"/>
+        <v>-1426.7855555555552</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="0"/>
+        <v>-1555.3166666666664</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="0"/>
+        <v>-1741.7027777777776</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="0"/>
+        <v>-1844.0594444444441</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22">
+        <v>5</v>
+      </c>
+      <c r="G22">
+        <v>6</v>
+      </c>
+      <c r="H22">
+        <v>7</v>
+      </c>
+      <c r="I22">
+        <v>8</v>
+      </c>
+      <c r="J22">
+        <v>9.81</v>
+      </c>
+      <c r="K22">
+        <v>11</v>
+      </c>
+      <c r="L22">
+        <v>12</v>
+      </c>
+      <c r="M22">
+        <v>13</v>
+      </c>
+      <c r="N22">
+        <v>14</v>
+      </c>
+      <c r="O22">
+        <v>15</v>
+      </c>
+      <c r="P22">
+        <v>16</v>
+      </c>
+      <c r="Q22">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>-275.23</v>
+      </c>
+      <c r="C23">
+        <v>-242.91</v>
+      </c>
+      <c r="D23">
+        <v>-134.72</v>
+      </c>
+      <c r="E23">
+        <v>-150.97999999999999</v>
+      </c>
+      <c r="F23">
+        <v>-815.37</v>
+      </c>
+      <c r="G23">
+        <v>-700.74</v>
+      </c>
+      <c r="H23">
+        <v>-709.36</v>
+      </c>
+      <c r="I23">
+        <v>-682.57</v>
+      </c>
+      <c r="J23">
+        <v>-913.48</v>
+      </c>
+      <c r="K23">
+        <v>-948.93</v>
+      </c>
+      <c r="L23">
+        <v>-1148.8800000000001</v>
+      </c>
+      <c r="M23">
+        <v>-1135.3</v>
+      </c>
+      <c r="N23">
+        <v>-1295.02</v>
+      </c>
+      <c r="O23">
+        <v>-1344.59</v>
+      </c>
+      <c r="P23">
+        <v>-1539.4</v>
+      </c>
+      <c r="Q23">
+        <v>-1694.02</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24">
+        <v>-63.71</v>
+      </c>
+      <c r="C24">
+        <v>-79.34</v>
+      </c>
+      <c r="D24">
+        <v>-71.709999999999994</v>
+      </c>
+      <c r="E24">
+        <v>-107.46</v>
+      </c>
+      <c r="F24">
+        <v>-662.35</v>
+      </c>
+      <c r="G24">
+        <v>-360.37</v>
+      </c>
+      <c r="H24">
+        <v>-363.8</v>
+      </c>
+      <c r="I24">
+        <v>-338.91</v>
+      </c>
+      <c r="J24">
+        <v>-351.74</v>
+      </c>
+      <c r="K24">
+        <v>-740.29</v>
+      </c>
+      <c r="L24">
+        <v>-729.01</v>
+      </c>
+      <c r="M24">
+        <v>-964.33</v>
+      </c>
+      <c r="N24">
+        <v>-826.55</v>
+      </c>
+      <c r="O24">
+        <v>-1287.4100000000001</v>
+      </c>
+      <c r="P24">
+        <v>-1439.09</v>
+      </c>
+      <c r="Q24">
+        <v>-1654.47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>-261.11</v>
+      </c>
+      <c r="C25">
+        <v>-259.39999999999998</v>
+      </c>
+      <c r="D25">
+        <v>-232.87</v>
+      </c>
+      <c r="E25">
+        <v>-482.79</v>
+      </c>
+      <c r="F25">
+        <v>-496.35</v>
+      </c>
+      <c r="G25">
+        <v>-447.32</v>
+      </c>
+      <c r="H25">
+        <v>-482.08</v>
+      </c>
+      <c r="I25">
+        <v>-662.74</v>
+      </c>
+      <c r="J25">
+        <v>-831.64</v>
+      </c>
+      <c r="K25">
+        <v>-965.16</v>
+      </c>
+      <c r="L25">
+        <v>-1043.54</v>
+      </c>
+      <c r="M25">
+        <v>-1173.49</v>
+      </c>
+      <c r="N25">
+        <v>-1281.57</v>
+      </c>
+      <c r="O25">
+        <v>-1170.3699999999999</v>
+      </c>
+      <c r="P25">
+        <v>-1585.31</v>
+      </c>
+      <c r="Q25">
+        <v>-1700.21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>-122.45</v>
+      </c>
+      <c r="C26">
+        <v>-188.19</v>
+      </c>
+      <c r="D26">
+        <v>-313.43</v>
+      </c>
+      <c r="E26">
+        <v>-320.75</v>
+      </c>
+      <c r="F26">
+        <v>-442.52</v>
+      </c>
+      <c r="G26">
+        <v>-421.35</v>
+      </c>
+      <c r="H26">
+        <v>-356.11</v>
+      </c>
+      <c r="I26">
+        <v>-345.63</v>
+      </c>
+      <c r="J26">
+        <v>-303.81</v>
+      </c>
+      <c r="K26">
+        <v>-322.44</v>
+      </c>
+      <c r="L26">
+        <v>-440.37</v>
+      </c>
+      <c r="M26">
+        <v>-1043.8900000000001</v>
+      </c>
+      <c r="N26">
+        <v>-1538.81</v>
+      </c>
+      <c r="O26">
+        <v>-1513.8</v>
+      </c>
+      <c r="P26">
+        <v>-1678.98</v>
+      </c>
+      <c r="Q26">
+        <v>-1853.78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27">
+        <v>-102.45</v>
+      </c>
+      <c r="C27">
+        <v>-79.069999999999993</v>
+      </c>
+      <c r="D27">
+        <v>-74.41</v>
+      </c>
+      <c r="E27">
+        <v>-117.78</v>
+      </c>
+      <c r="F27">
+        <v>-501.02</v>
+      </c>
+      <c r="G27">
+        <v>-306.77999999999997</v>
+      </c>
+      <c r="H27">
+        <v>-426.89</v>
+      </c>
+      <c r="I27">
+        <v>-289.20999999999998</v>
+      </c>
+      <c r="J27">
+        <v>-327.29000000000002</v>
+      </c>
+      <c r="K27">
+        <v>-568.05999999999995</v>
+      </c>
+      <c r="L27">
+        <v>-650.11</v>
+      </c>
+      <c r="M27">
+        <v>-758.64</v>
+      </c>
+      <c r="N27">
+        <v>-882.11</v>
+      </c>
+      <c r="O27">
+        <v>-915.95</v>
+      </c>
+      <c r="P27">
+        <v>-1393.81</v>
+      </c>
+      <c r="Q27">
+        <v>-1571.79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28">
+        <v>-506.76</v>
+      </c>
+      <c r="C28">
+        <v>-813.67</v>
+      </c>
+      <c r="D28">
+        <v>-880.16</v>
+      </c>
+      <c r="E28">
+        <v>-938.72</v>
+      </c>
+      <c r="F28">
+        <v>-764.31</v>
+      </c>
+      <c r="G28">
+        <v>-683.06</v>
+      </c>
+      <c r="H28">
+        <v>-559.30999999999995</v>
+      </c>
+      <c r="I28">
+        <v>-769.61</v>
+      </c>
+      <c r="J28">
+        <v>-845.07</v>
+      </c>
+      <c r="K28">
+        <v>-890.64</v>
+      </c>
+      <c r="L28">
+        <v>-1367.43</v>
+      </c>
+      <c r="M28">
+        <v>-1567.2</v>
+      </c>
+      <c r="N28">
+        <v>-1690.3</v>
+      </c>
+      <c r="O28">
+        <v>-1772.79</v>
+      </c>
+      <c r="P28">
+        <v>-1895.94</v>
+      </c>
+      <c r="Q28">
+        <v>-1972.24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29">
+        <v>-253.51</v>
+      </c>
+      <c r="C29">
+        <v>-259.76</v>
+      </c>
+      <c r="D29">
+        <v>-313.29000000000002</v>
+      </c>
+      <c r="E29">
+        <v>-393.04</v>
+      </c>
+      <c r="F29">
+        <v>-319.36</v>
+      </c>
+      <c r="G29">
+        <v>-373.86</v>
+      </c>
+      <c r="H29">
+        <v>-435.04</v>
+      </c>
+      <c r="I29">
+        <v>-472.52</v>
+      </c>
+      <c r="J29">
+        <v>-542.74</v>
+      </c>
+      <c r="K29">
+        <v>-622.55999999999995</v>
+      </c>
+      <c r="L29">
+        <v>-967.4</v>
+      </c>
+      <c r="M29">
+        <v>-1658.92</v>
+      </c>
+      <c r="N29">
+        <v>-1788.35</v>
+      </c>
+      <c r="O29">
+        <v>-1919.42</v>
+      </c>
+      <c r="P29">
+        <v>-1947.23</v>
+      </c>
+      <c r="Q29">
+        <v>-1922.15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30">
+        <v>-143.72</v>
+      </c>
+      <c r="C30">
+        <v>-62.61</v>
+      </c>
+      <c r="D30">
+        <v>-78.73</v>
+      </c>
+      <c r="E30">
+        <v>-86.92</v>
+      </c>
+      <c r="F30">
+        <v>-367.21</v>
+      </c>
+      <c r="G30">
+        <v>-420.77</v>
+      </c>
+      <c r="H30">
+        <v>-377.73</v>
+      </c>
+      <c r="I30">
+        <v>-212.97</v>
+      </c>
+      <c r="J30">
+        <v>-339.49</v>
+      </c>
+      <c r="K30">
+        <v>-493.35</v>
+      </c>
+      <c r="L30">
+        <v>-466.17</v>
+      </c>
+      <c r="M30">
+        <v>-602.4</v>
+      </c>
+      <c r="N30">
+        <v>-680.98</v>
+      </c>
+      <c r="O30">
+        <v>-696.48</v>
+      </c>
+      <c r="P30">
+        <v>-1358.77</v>
+      </c>
+      <c r="Q30">
+        <v>-1519.34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31">
+        <v>-777.3</v>
+      </c>
+      <c r="C31">
+        <v>-914.73</v>
+      </c>
+      <c r="D31">
+        <v>-822.22</v>
+      </c>
+      <c r="E31">
+        <v>-979.89</v>
+      </c>
+      <c r="F31">
+        <v>-872.65</v>
+      </c>
+      <c r="G31">
+        <v>-1091.69</v>
+      </c>
+      <c r="H31">
+        <v>-966.03</v>
+      </c>
+      <c r="I31">
+        <v>-715.85</v>
+      </c>
+      <c r="J31">
+        <v>-485.38</v>
+      </c>
+      <c r="K31">
+        <v>-1391.83</v>
+      </c>
+      <c r="L31">
+        <v>-1654.53</v>
+      </c>
+      <c r="M31">
+        <v>-1883.92</v>
+      </c>
+      <c r="N31">
+        <v>-1719.65</v>
+      </c>
+      <c r="O31">
+        <v>-1885.24</v>
+      </c>
+      <c r="P31">
+        <v>-2013.94</v>
+      </c>
+      <c r="Q31">
+        <v>-2022.45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32">
+        <v>-84.64</v>
+      </c>
+      <c r="C32">
+        <v>-77.209999999999994</v>
+      </c>
+      <c r="D32">
+        <v>-97.52</v>
+      </c>
+      <c r="E32">
+        <v>-176.59</v>
+      </c>
+      <c r="F32">
+        <v>-534.52</v>
+      </c>
+      <c r="G32">
+        <v>-394.67</v>
+      </c>
+      <c r="H32">
+        <v>-431.43</v>
+      </c>
+      <c r="I32">
+        <v>-332.02</v>
+      </c>
+      <c r="J32">
+        <v>-472.42</v>
+      </c>
+      <c r="K32">
+        <v>-313.89999999999998</v>
+      </c>
+      <c r="L32">
+        <v>-259.23</v>
+      </c>
+      <c r="M32">
+        <v>-359.09</v>
+      </c>
+      <c r="N32">
+        <v>-1090.83</v>
+      </c>
+      <c r="O32">
+        <v>-1540.24</v>
+      </c>
+      <c r="P32">
+        <v>-1724.38</v>
+      </c>
+      <c r="Q32">
+        <v>-1686.35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33">
+        <v>-735.9</v>
+      </c>
+      <c r="C33">
+        <v>-757.48</v>
+      </c>
+      <c r="D33">
+        <v>-806.37</v>
+      </c>
+      <c r="E33">
+        <v>-574.64</v>
+      </c>
+      <c r="F33">
+        <v>-586.11</v>
+      </c>
+      <c r="G33">
+        <v>-543.74</v>
+      </c>
+      <c r="H33">
+        <v>-490.72</v>
+      </c>
+      <c r="I33">
+        <v>-438.39</v>
+      </c>
+      <c r="J33">
+        <v>-449.81</v>
+      </c>
+      <c r="K33">
+        <v>-428.61</v>
+      </c>
+      <c r="L33">
+        <v>-769.46</v>
+      </c>
+      <c r="M33">
+        <v>-1307.49</v>
+      </c>
+      <c r="N33">
+        <v>-1717.2</v>
+      </c>
+      <c r="O33">
+        <v>-1833.18</v>
+      </c>
+      <c r="P33">
+        <v>-1922.43</v>
+      </c>
+      <c r="Q33">
+        <v>-1955.6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34">
+        <v>-199.75</v>
+      </c>
+      <c r="C34">
+        <v>-121.54</v>
+      </c>
+      <c r="D34">
+        <v>-221.3</v>
+      </c>
+      <c r="E34">
+        <v>-185.66</v>
+      </c>
+      <c r="F34">
+        <v>-602.98</v>
+      </c>
+      <c r="G34">
+        <v>-689.44</v>
+      </c>
+      <c r="H34">
+        <v>-679.79</v>
+      </c>
+      <c r="I34">
+        <v>-870.84</v>
+      </c>
+      <c r="J34">
+        <v>-1055.8</v>
+      </c>
+      <c r="K34">
+        <v>-1147.07</v>
+      </c>
+      <c r="L34">
+        <v>-1278.43</v>
+      </c>
+      <c r="M34">
+        <v>-1220.82</v>
+      </c>
+      <c r="N34">
+        <v>-1226.27</v>
+      </c>
+      <c r="O34">
+        <v>-1281.83</v>
+      </c>
+      <c r="P34">
+        <v>-1403.98</v>
+      </c>
+      <c r="Q34">
+        <v>-1589.37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35">
+        <v>-649.85</v>
+      </c>
+      <c r="C35">
+        <v>-573.73</v>
+      </c>
+      <c r="D35">
+        <v>-666.32</v>
+      </c>
+      <c r="E35">
+        <v>-718.45</v>
+      </c>
+      <c r="F35">
+        <v>-610.42999999999995</v>
+      </c>
+      <c r="G35">
+        <v>-511.37</v>
+      </c>
+      <c r="H35">
+        <v>-394.75</v>
+      </c>
+      <c r="I35">
+        <v>-390.88</v>
+      </c>
+      <c r="J35">
+        <v>-215.67</v>
+      </c>
+      <c r="K35">
+        <v>-256.58</v>
+      </c>
+      <c r="L35">
+        <v>-402.68</v>
+      </c>
+      <c r="M35">
+        <v>-1338.68</v>
+      </c>
+      <c r="N35">
+        <v>-1588.12</v>
+      </c>
+      <c r="O35">
+        <v>-1705.61</v>
+      </c>
+      <c r="P35">
+        <v>-1866.84</v>
+      </c>
+      <c r="Q35">
+        <v>-1989.53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36">
+        <v>-255.37</v>
+      </c>
+      <c r="C36">
+        <v>-208.79</v>
+      </c>
+      <c r="D36">
+        <v>-211.47</v>
+      </c>
+      <c r="E36">
+        <v>-189.68</v>
+      </c>
+      <c r="F36">
+        <v>-230.32</v>
+      </c>
+      <c r="G36">
+        <v>-223.29</v>
+      </c>
+      <c r="H36">
+        <v>-232.27</v>
+      </c>
+      <c r="I36">
+        <v>-396.58</v>
+      </c>
+      <c r="J36">
+        <v>-314.38</v>
+      </c>
+      <c r="K36">
+        <v>-392.85</v>
+      </c>
+      <c r="L36">
+        <v>-662.52</v>
+      </c>
+      <c r="M36">
+        <v>-1159.08</v>
+      </c>
+      <c r="N36">
+        <v>-1354.06</v>
+      </c>
+      <c r="O36">
+        <v>-1666.42</v>
+      </c>
+      <c r="P36">
+        <v>-1833.84</v>
+      </c>
+      <c r="Q36">
+        <v>-1925.19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37">
+        <v>-134.61000000000001</v>
+      </c>
+      <c r="C37">
+        <v>-143.61000000000001</v>
+      </c>
+      <c r="D37">
+        <v>-129.91999999999999</v>
+      </c>
+      <c r="E37">
+        <v>-152.12</v>
+      </c>
+      <c r="F37">
+        <v>-160.94</v>
+      </c>
+      <c r="G37">
+        <v>-165.41</v>
+      </c>
+      <c r="H37">
+        <v>-178.39</v>
+      </c>
+      <c r="I37">
+        <v>-198.05</v>
+      </c>
+      <c r="J37">
+        <v>-245.34</v>
+      </c>
+      <c r="K37">
+        <v>-297.76</v>
+      </c>
+      <c r="L37">
+        <v>-397.98</v>
+      </c>
+      <c r="M37">
+        <v>-1401.08</v>
+      </c>
+      <c r="N37">
+        <v>-1545.8</v>
+      </c>
+      <c r="O37">
+        <v>-1657.87</v>
+      </c>
+      <c r="P37">
+        <v>-1744.01</v>
+      </c>
+      <c r="Q37">
+        <v>-1940.92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38">
+        <v>-109.73</v>
+      </c>
+      <c r="C38">
+        <v>-154.09</v>
+      </c>
+      <c r="D38">
+        <v>-521.14</v>
+      </c>
+      <c r="E38">
+        <v>-522.01</v>
+      </c>
+      <c r="F38">
+        <v>-535.98</v>
+      </c>
+      <c r="G38">
+        <v>-497.87</v>
+      </c>
+      <c r="H38">
+        <v>-513.01</v>
+      </c>
+      <c r="I38">
+        <v>-448.24</v>
+      </c>
+      <c r="J38">
+        <v>-461.42</v>
+      </c>
+      <c r="K38">
+        <v>-487.28</v>
+      </c>
+      <c r="L38">
+        <v>-582.30999999999995</v>
+      </c>
+      <c r="M38">
+        <v>-623.04999999999995</v>
+      </c>
+      <c r="N38">
+        <v>-1488.05</v>
+      </c>
+      <c r="O38">
+        <v>-1664.75</v>
+      </c>
+      <c r="P38">
+        <v>-1765.01</v>
+      </c>
+      <c r="Q38">
+        <v>-1887.79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B39">
+        <f>AVERAGE(B23:B38)</f>
+        <v>-292.25562499999995</v>
+      </c>
+      <c r="C39">
+        <f t="shared" ref="C39:Q39" si="1">AVERAGE(C23:C38)</f>
+        <v>-308.50812499999995</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="1"/>
+        <v>-348.47375000000005</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="1"/>
+        <v>-381.09250000000003</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="1"/>
+        <v>-531.40125</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>-489.48312500000003</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="1"/>
+        <v>-474.79437500000006</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="1"/>
+        <v>-472.81312500000007</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="1"/>
+        <v>-509.71750000000009</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="1"/>
+        <v>-641.70687500000008</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="1"/>
+        <v>-801.25312500000007</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="1"/>
+        <v>-1137.3362500000001</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="1"/>
+        <v>-1357.1043749999999</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="1"/>
+        <v>-1490.996875</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="1"/>
+        <v>-1694.5599999999997</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="1"/>
+        <v>-1805.3249999999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
wirte grav 11 and 9.81 to excel
</commit_message>
<xml_diff>
--- a/pendulum/work_on_memory/memory_grav.xlsx
+++ b/pendulum/work_on_memory/memory_grav.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="9.81" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Outliers" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="13" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="14" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="11" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -427,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q39"/>
+  <dimension ref="A1:Q46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R30" sqref="R30"/>
@@ -2545,6 +2546,391 @@
       <c r="Q39">
         <f>AVERAGE(Q23:Q38)</f>
         <v/>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>sub(sub(memProtectedDiv(cos(cos(sub(0, read(a0, protectedLog(a2))))), sub(read(a0, memProtectedDiv(a1, protectedLog(read(a0, protectedLog(0))))), a2)), a2), write(a0, write(a0, a1, 0), sin(sin(a2))))</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>-53.36</v>
+      </c>
+      <c r="C40" t="n">
+        <v>-57.29</v>
+      </c>
+      <c r="D40" t="n">
+        <v>-63.55</v>
+      </c>
+      <c r="E40" t="n">
+        <v>-101.51</v>
+      </c>
+      <c r="F40" t="n">
+        <v>-662.36</v>
+      </c>
+      <c r="G40" t="n">
+        <v>-445.79</v>
+      </c>
+      <c r="H40" t="n">
+        <v>-371.19</v>
+      </c>
+      <c r="I40" t="n">
+        <v>-376.79</v>
+      </c>
+      <c r="J40" t="n">
+        <v>-330.73</v>
+      </c>
+      <c r="K40" t="n">
+        <v>-625.26</v>
+      </c>
+      <c r="L40" t="n">
+        <v>-989.35</v>
+      </c>
+      <c r="M40" t="n">
+        <v>-897.12</v>
+      </c>
+      <c r="N40" t="n">
+        <v>-722.1</v>
+      </c>
+      <c r="O40" t="n">
+        <v>-1207.74</v>
+      </c>
+      <c r="P40" t="n">
+        <v>-1332.14</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>-1483.36</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>sub(read(a0, 0), add(add(add(add(write(a0, a1, add(memProtectedDiv(add(add(write(a0, read(a0, add(0, add(write(a0, a2, a2), read(a0, cos(a2))))), a1), a1), a1), conditional(a2, a1)), a1)), limit(a1, 0, a2)), a2), sin(read(a0, a1))), a2))</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>-114.66</v>
+      </c>
+      <c r="C41" t="n">
+        <v>-103.36</v>
+      </c>
+      <c r="D41" t="n">
+        <v>-111.13</v>
+      </c>
+      <c r="E41" t="n">
+        <v>-210.32</v>
+      </c>
+      <c r="F41" t="n">
+        <v>-279.37</v>
+      </c>
+      <c r="G41" t="n">
+        <v>-254.06</v>
+      </c>
+      <c r="H41" t="n">
+        <v>-250.68</v>
+      </c>
+      <c r="I41" t="n">
+        <v>-268.75</v>
+      </c>
+      <c r="J41" t="n">
+        <v>-269.74</v>
+      </c>
+      <c r="K41" t="n">
+        <v>-335.02</v>
+      </c>
+      <c r="L41" t="n">
+        <v>-371.18</v>
+      </c>
+      <c r="M41" t="n">
+        <v>-540.4299999999999</v>
+      </c>
+      <c r="N41" t="n">
+        <v>-712.85</v>
+      </c>
+      <c r="O41" t="n">
+        <v>-1411.94</v>
+      </c>
+      <c r="P41" t="n">
+        <v>-1595.65</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>-1710.47</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>sub(a1, add(memProtectedDiv(cos(0), limit(add(abs(a1), 0), 0, sub(sin(limit(a1, a2, memProtectedDiv(a2, sin(a1)))), read(a0, a2)))), write(a0, protectedLog(read(a0, write(a0, a1, protectedLog(a1)))), a2)))</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>-538.6900000000001</v>
+      </c>
+      <c r="C42" t="n">
+        <v>-584.9400000000001</v>
+      </c>
+      <c r="D42" t="n">
+        <v>-575.12</v>
+      </c>
+      <c r="E42" t="n">
+        <v>-669.16</v>
+      </c>
+      <c r="F42" t="n">
+        <v>-803.64</v>
+      </c>
+      <c r="G42" t="n">
+        <v>-712.4400000000001</v>
+      </c>
+      <c r="H42" t="n">
+        <v>-648.76</v>
+      </c>
+      <c r="I42" t="n">
+        <v>-547.39</v>
+      </c>
+      <c r="J42" t="n">
+        <v>-211.68</v>
+      </c>
+      <c r="K42" t="n">
+        <v>-224.8</v>
+      </c>
+      <c r="L42" t="n">
+        <v>-335.98</v>
+      </c>
+      <c r="M42" t="n">
+        <v>-1452.27</v>
+      </c>
+      <c r="N42" t="n">
+        <v>-1711.52</v>
+      </c>
+      <c r="O42" t="n">
+        <v>-1864.67</v>
+      </c>
+      <c r="P42" t="n">
+        <v>-1920.95</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>-2089.28</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>limit(conditional(a2, read(a0, a1)), write(a0, a2, a2), memProtectedDiv(memProtectedDiv(a2, cos(add(a1, a2))), protectedLog(sin(conditional(a1, memProtectedDiv(read(a0, limit(a1, a1, conditional(a1, memProtectedDiv(limit(abs(a1), 0, a2), memProtectedDiv(sub(read(a0, 0), limit(sub(a2, read(a0, read(a0, a2))), a1, a2)), abs(conditional(a2, 0))))))), a1))))))</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>-483.24</v>
+      </c>
+      <c r="C43" t="n">
+        <v>-500.67</v>
+      </c>
+      <c r="D43" t="n">
+        <v>-542.27</v>
+      </c>
+      <c r="E43" t="n">
+        <v>-631.86</v>
+      </c>
+      <c r="F43" t="n">
+        <v>-610.58</v>
+      </c>
+      <c r="G43" t="n">
+        <v>-613.95</v>
+      </c>
+      <c r="H43" t="n">
+        <v>-676.38</v>
+      </c>
+      <c r="I43" t="n">
+        <v>-794.3200000000001</v>
+      </c>
+      <c r="J43" t="n">
+        <v>-788.9299999999999</v>
+      </c>
+      <c r="K43" t="n">
+        <v>-977.5599999999999</v>
+      </c>
+      <c r="L43" t="n">
+        <v>-1490.9</v>
+      </c>
+      <c r="M43" t="n">
+        <v>-1650.19</v>
+      </c>
+      <c r="N43" t="n">
+        <v>-1812.14</v>
+      </c>
+      <c r="O43" t="n">
+        <v>-1919.24</v>
+      </c>
+      <c r="P43" t="n">
+        <v>-1994.35</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>-2055.18</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>sub(memProtectedDiv(sub(protectedLog(0), memProtectedDiv(memProtectedDiv(a1, sub(0, a1)), memProtectedDiv(sub(read(a0, a2), a2), cos(read(a0, a2))))), abs(write(a0, a1, sin(write(a0, 0, sin(a2)))))), a1)</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>-56.03</v>
+      </c>
+      <c r="C44" t="n">
+        <v>-55.73</v>
+      </c>
+      <c r="D44" t="n">
+        <v>-67.84999999999999</v>
+      </c>
+      <c r="E44" t="n">
+        <v>-114.04</v>
+      </c>
+      <c r="F44" t="n">
+        <v>-598.5700000000001</v>
+      </c>
+      <c r="G44" t="n">
+        <v>-565.79</v>
+      </c>
+      <c r="H44" t="n">
+        <v>-314.34</v>
+      </c>
+      <c r="I44" t="n">
+        <v>-260.4</v>
+      </c>
+      <c r="J44" t="n">
+        <v>-404.53</v>
+      </c>
+      <c r="K44" t="n">
+        <v>-682.04</v>
+      </c>
+      <c r="L44" t="n">
+        <v>-1085.91</v>
+      </c>
+      <c r="M44" t="n">
+        <v>-826.71</v>
+      </c>
+      <c r="N44" t="n">
+        <v>-750.12</v>
+      </c>
+      <c r="O44" t="n">
+        <v>-1210.49</v>
+      </c>
+      <c r="P44" t="n">
+        <v>-1341.26</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>-1476.33</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>sub(a1, memProtectedDiv(conditional(add(a2, read(a0, 0)), write(a0, write(a0, conditional(0, a2), 0), memProtectedDiv(add(a1, a1), a2))), a2))</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>-98.12</v>
+      </c>
+      <c r="C45" t="n">
+        <v>-128.26</v>
+      </c>
+      <c r="D45" t="n">
+        <v>-143.32</v>
+      </c>
+      <c r="E45" t="n">
+        <v>-158.86</v>
+      </c>
+      <c r="F45" t="n">
+        <v>-166.58</v>
+      </c>
+      <c r="G45" t="n">
+        <v>-172.25</v>
+      </c>
+      <c r="H45" t="n">
+        <v>-189.62</v>
+      </c>
+      <c r="I45" t="n">
+        <v>-200.35</v>
+      </c>
+      <c r="J45" t="n">
+        <v>-230.49</v>
+      </c>
+      <c r="K45" t="n">
+        <v>-293.33</v>
+      </c>
+      <c r="L45" t="n">
+        <v>-597.52</v>
+      </c>
+      <c r="M45" t="n">
+        <v>-932.99</v>
+      </c>
+      <c r="N45" t="n">
+        <v>-1051.29</v>
+      </c>
+      <c r="O45" t="n">
+        <v>-1260.92</v>
+      </c>
+      <c r="P45" t="n">
+        <v>-1583.19</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>-1751.11</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>conditional(read(a0, 0), write(a0, limit(a1, a1, limit(a2, a2, 0)), limit(a1, add(add(write(a0, a1, limit(a1, add(a2, memProtectedDiv(a1, a1)), a1)), memProtectedDiv(a1, a1)), cos(limit(a1, 0, sub(0, a2)))), 0)))</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>-580.48</v>
+      </c>
+      <c r="C46" t="n">
+        <v>-782.6799999999999</v>
+      </c>
+      <c r="D46" t="n">
+        <v>-833.86</v>
+      </c>
+      <c r="E46" t="n">
+        <v>-757.6</v>
+      </c>
+      <c r="F46" t="n">
+        <v>-523.5599999999999</v>
+      </c>
+      <c r="G46" t="n">
+        <v>-683.97</v>
+      </c>
+      <c r="H46" t="n">
+        <v>-655.3099999999999</v>
+      </c>
+      <c r="I46" t="n">
+        <v>-484.37</v>
+      </c>
+      <c r="J46" t="n">
+        <v>-523.1799999999999</v>
+      </c>
+      <c r="K46" t="n">
+        <v>-843.04</v>
+      </c>
+      <c r="L46" t="n">
+        <v>-1330.07</v>
+      </c>
+      <c r="M46" t="n">
+        <v>-1551.47</v>
+      </c>
+      <c r="N46" t="n">
+        <v>-1669.18</v>
+      </c>
+      <c r="O46" t="n">
+        <v>-1768.6</v>
+      </c>
+      <c r="P46" t="n">
+        <v>-1908.3</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>-1955.64</v>
       </c>
     </row>
   </sheetData>
@@ -3603,4 +3989,683 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sub(add(a1, add(limit(a1, 0, read(a0, a1)), read(a0, a2))), write(a0, memProtectedDiv(a2, add(0, protectedLog(a1))), memProtectedDiv(sub(0, write(a0, 0, abs(write(a0, cos(abs(sub(a2, a1))), memProtectedDiv(a1, a2))))), add(sin(conditional(a2, write(a0, a2, add(a2, a2)))), limit(limit(0, memProtectedDiv(sin(a1), a1), sub(a1, a1)), 0, a2)))))</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>-357.43</v>
+      </c>
+      <c r="C1" t="n">
+        <v>-274.91</v>
+      </c>
+      <c r="D1" t="n">
+        <v>-238.23</v>
+      </c>
+      <c r="E1" t="n">
+        <v>-251.93</v>
+      </c>
+      <c r="F1" t="n">
+        <v>-331.23</v>
+      </c>
+      <c r="G1" t="n">
+        <v>-336.47</v>
+      </c>
+      <c r="H1" t="n">
+        <v>-283.45</v>
+      </c>
+      <c r="I1" t="n">
+        <v>-291.53</v>
+      </c>
+      <c r="J1" t="n">
+        <v>-283.39</v>
+      </c>
+      <c r="K1" t="n">
+        <v>-272.66</v>
+      </c>
+      <c r="L1" t="n">
+        <v>-342.42</v>
+      </c>
+      <c r="M1" t="n">
+        <v>-345.37</v>
+      </c>
+      <c r="N1" t="n">
+        <v>-1502.48</v>
+      </c>
+      <c r="O1" t="n">
+        <v>-1685.33</v>
+      </c>
+      <c r="P1" t="n">
+        <v>-1778.3</v>
+      </c>
+      <c r="Q1" t="n">
+        <v>-1931.88</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>memProtectedDiv(sub(sin(read(a0, a1)), write(a0, 0, sin(a2))), abs(memProtectedDiv(sub(a2, sin(a2)), memProtectedDiv(sin(a1), read(a0, protectedLog(a1))))))</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-238.18</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-276.72</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-319.23</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-441.98</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-596.5700000000001</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-644.6799999999999</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-591.77</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-730.21</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-755.5700000000001</v>
+      </c>
+      <c r="K2" t="n">
+        <v>-296.64</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-382.86</v>
+      </c>
+      <c r="M2" t="n">
+        <v>-1297.22</v>
+      </c>
+      <c r="N2" t="n">
+        <v>-1489.24</v>
+      </c>
+      <c r="O2" t="n">
+        <v>-1680.67</v>
+      </c>
+      <c r="P2" t="n">
+        <v>-1829.78</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>-1931.78</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>sub(add(add(read(a0, protectedLog(abs(sin(a2)))), conditional(0, abs(a2))), sub(a2, memProtectedDiv(add(conditional(a1, 0), a1), a2))), write(a0, 0, sub(0, memProtectedDiv(add(write(a0, a1, conditional(memProtectedDiv(a1, a2), a1)), read(a0, a2)), a2))))</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>-852.38</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-793.55</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-931.95</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-828.66</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-935.8099999999999</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-966.9400000000001</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-827.02</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-801.09</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-341.52</v>
+      </c>
+      <c r="K3" t="n">
+        <v>-265.79</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-380.61</v>
+      </c>
+      <c r="M3" t="n">
+        <v>-1503.4</v>
+      </c>
+      <c r="N3" t="n">
+        <v>-1720.24</v>
+      </c>
+      <c r="O3" t="n">
+        <v>-1843.7</v>
+      </c>
+      <c r="P3" t="n">
+        <v>-1917.37</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>-1979.78</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>limit(add(0, a2), conditional(a2, read(a0, limit(a2, a1, sin(a2)))), add(sub(a2, sub(memProtectedDiv(add(a1, read(a0, write(a0, 0, limit(a2, a1, a2)))), a2), sub(conditional(a1, a2), a1))), write(a0, memProtectedDiv(a2, 0), a2)))</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>-1641.73</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-1811.87</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-2144.95</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-2090.29</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-2016.75</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-1949.89</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-1856.26</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-1739.01</v>
+      </c>
+      <c r="J4" t="n">
+        <v>-1517.65</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-1073.6</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-1566.47</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-1762.24</v>
+      </c>
+      <c r="N4" t="n">
+        <v>-1887.93</v>
+      </c>
+      <c r="O4" t="n">
+        <v>-1989.55</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-2057.86</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>-2126.05</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>sub(add(limit(a1, a2, a1), read(a0, add(a2, a2))), write(a0, sin(a1), add(memProtectedDiv(a1, conditional(a2, a1)), add(add(add(memProtectedDiv(0, 0), add(a2, a2)), add(0, a2)), write(a0, write(a0, a1, 0), a2)))))</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-1879.12</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-1989.46</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-1880.64</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-1897.77</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-1848.04</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-1739.85</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-1674.16</v>
+      </c>
+      <c r="I5" t="n">
+        <v>-1477.89</v>
+      </c>
+      <c r="J5" t="n">
+        <v>-1336.82</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-394.05</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-1247.14</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-1658.71</v>
+      </c>
+      <c r="N5" t="n">
+        <v>-1812.08</v>
+      </c>
+      <c r="O5" t="n">
+        <v>-1925.99</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-2003.5</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-2053.11</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>sub(read(a0, a1), write(a0, a1, memProtectedDiv(add(sub(limit(0, limit(a1, 0, memProtectedDiv(sub(a1, protectedLog(a1)), protectedLog(a1))), add(sub(a1, abs(sub(memProtectedDiv(a1, a2), a2))), protectedLog(limit(0, abs(sub(write(a0, a2, a2), add(sin(a2), 0))), a2)))), abs(sub(memProtectedDiv(a1, a2), read(a0, a1)))), protectedLog(limit(a2, 0, memProtectedDiv(add(sub(add(a1, a2), abs(sub(memProtectedDiv(a1, abs(sub(abs(0), add(sin(a2), 0)))), a2))), protectedLog(read(a0, read(a0, a2)))), a1)))), a2)))</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-2015.15</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-2062.02</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-2087.44</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-2132.41</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-2071.12</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-2049.1</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-1959.36</v>
+      </c>
+      <c r="I6" t="n">
+        <v>-1820.44</v>
+      </c>
+      <c r="J6" t="n">
+        <v>-1544.35</v>
+      </c>
+      <c r="K6" t="n">
+        <v>-569.38</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-1099.77</v>
+      </c>
+      <c r="M6" t="n">
+        <v>-1477.01</v>
+      </c>
+      <c r="N6" t="n">
+        <v>-1646.3</v>
+      </c>
+      <c r="O6" t="n">
+        <v>-1770.55</v>
+      </c>
+      <c r="P6" t="n">
+        <v>-1876.49</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>-1976.36</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>sub(memProtectedDiv(conditional(read(a0, cos(sub(0, a2))), write(a0, write(a0, add(a2, read(a0, 0)), protectedLog(write(a0, read(a0, 0), a1))), conditional(a2, conditional(read(a0, 0), cos(add(protectedLog(sub(a1, 0)), a1)))))), add(a2, memProtectedDiv(a2, 0))), sin(cos(a1)))</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>-1761.88</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-1665.08</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-1713.05</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-1986.6</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-2074.95</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-1957.69</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-1946.86</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-1887.12</v>
+      </c>
+      <c r="J7" t="n">
+        <v>-1532.77</v>
+      </c>
+      <c r="K7" t="n">
+        <v>-596.8</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-1065.85</v>
+      </c>
+      <c r="M7" t="n">
+        <v>-1663.95</v>
+      </c>
+      <c r="N7" t="n">
+        <v>-1784.88</v>
+      </c>
+      <c r="O7" t="n">
+        <v>-1872.64</v>
+      </c>
+      <c r="P7" t="n">
+        <v>-1959.12</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>-2045.08</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>sub(read(a0, a2), write(a0, a2, write(a0, write(a0, a2, write(a0, a1, add(write(a0, write(a0, a2, write(a0, a2, add(write(a0, protectedLog(a2), add(0, memProtectedDiv(memProtectedDiv(a2, protectedLog(cos(a2))), conditional(abs(a2), 0)))), memProtectedDiv(abs(a2), conditional(a1, 0))))), add(memProtectedDiv(a1, 0), memProtectedDiv(memProtectedDiv(a2, conditional(limit(a2, a2, 0), a2)), conditional(a2, 0)))), memProtectedDiv(sub(a2, memProtectedDiv(a2, a1)), conditional(a1, protectedLog(a1)))))), add(write(a0, a2, add(0, memProtectedDiv(memProtectedDiv(a2, protectedLog(cos(a2))), conditional(a2, limit(sin(a1), conditional(0, sub(cos(0), abs(a1))), sin(0)))))), memProtectedDiv(sub(a2, memProtectedDiv(a2, a1)), abs(a1))))))</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-2049.74</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-2268.23</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-2175.2</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-2164.05</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-2106.42</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-2140.33</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-2005.4</v>
+      </c>
+      <c r="I8" t="n">
+        <v>-1777.37</v>
+      </c>
+      <c r="J8" t="n">
+        <v>-1529.51</v>
+      </c>
+      <c r="K8" t="n">
+        <v>-634.6799999999999</v>
+      </c>
+      <c r="L8" t="n">
+        <v>-1142.34</v>
+      </c>
+      <c r="M8" t="n">
+        <v>-1482.94</v>
+      </c>
+      <c r="N8" t="n">
+        <v>-1626.38</v>
+      </c>
+      <c r="O8" t="n">
+        <v>-1766.23</v>
+      </c>
+      <c r="P8" t="n">
+        <v>-1868.6</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>-1964.6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>sub(sin(read(a0, 0)), limit(conditional(read(a0, a2), write(a0, cos(sub(a1, 0)), memProtectedDiv(cos(0), a2))), 0, read(a0, 0)))</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-625.24</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-694.03</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-776.71</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-886.64</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-968.71</v>
+      </c>
+      <c r="G9" t="n">
+        <v>-1064.95</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-1081.84</v>
+      </c>
+      <c r="I9" t="n">
+        <v>-1209.34</v>
+      </c>
+      <c r="J9" t="n">
+        <v>-1033.25</v>
+      </c>
+      <c r="K9" t="n">
+        <v>-417.1</v>
+      </c>
+      <c r="L9" t="n">
+        <v>-1390.01</v>
+      </c>
+      <c r="M9" t="n">
+        <v>-1567.33</v>
+      </c>
+      <c r="N9" t="n">
+        <v>-1632.22</v>
+      </c>
+      <c r="O9" t="n">
+        <v>-1771.4</v>
+      </c>
+      <c r="P9" t="n">
+        <v>-1923.03</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>-2006.75</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>sub(add(read(a0, 0), conditional(a1, add(a1, write(a0, limit(read(a0, abs(cos(a1))), abs(memProtectedDiv(limit(sin(a1), memProtectedDiv(a2, conditional(a1, write(a0, 0, read(a0, 0)))), sub(a1, 0)), sub(a1, sub(limit(sin(read(a0, cos(a1))), memProtectedDiv(a2, a1), sub(0, 0)), write(a0, a1, a1))))), limit(limit(memProtectedDiv(a1, a2), 0, abs(read(a0, a1))), 0, limit(limit(a1, 0, a1), abs(0), a2))), a2)))), write(a0, add(0, 0), memProtectedDiv(a1, conditional(a2, write(a0, a2, a1)))))</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>-579.83</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-759.05</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-724.01</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-888.39</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-893.73</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-1043.51</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-1019.99</v>
+      </c>
+      <c r="I10" t="n">
+        <v>-1061.83</v>
+      </c>
+      <c r="J10" t="n">
+        <v>-1000.21</v>
+      </c>
+      <c r="K10" t="n">
+        <v>-431.7</v>
+      </c>
+      <c r="L10" t="n">
+        <v>-1349.95</v>
+      </c>
+      <c r="M10" t="n">
+        <v>-1564.93</v>
+      </c>
+      <c r="N10" t="n">
+        <v>-1713.35</v>
+      </c>
+      <c r="O10" t="n">
+        <v>-1823.08</v>
+      </c>
+      <c r="P10" t="n">
+        <v>-1904.3</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>-2047.9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>add(limit(a2, read(a0, a1), memProtectedDiv(memProtectedDiv(sub(a2, conditional(a1, sub(conditional(a2, cos(abs(a1))), protectedLog(sub(a2, a2))))), a1), a2)), cos(limit(cos(a1), a1, write(a0, conditional(0, a2), a2))))</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>-1838.53</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-1986.86</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-1820.35</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-1859.26</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-1729.15</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-1689.91</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-1554.81</v>
+      </c>
+      <c r="I11" t="n">
+        <v>-1563.12</v>
+      </c>
+      <c r="J11" t="n">
+        <v>-1360.68</v>
+      </c>
+      <c r="K11" t="n">
+        <v>-387.64</v>
+      </c>
+      <c r="L11" t="n">
+        <v>-1593.74</v>
+      </c>
+      <c r="M11" t="n">
+        <v>-1769.09</v>
+      </c>
+      <c r="N11" t="n">
+        <v>-1864.14</v>
+      </c>
+      <c r="O11" t="n">
+        <v>-1942.86</v>
+      </c>
+      <c r="P11" t="n">
+        <v>-1999.86</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>-2082.54</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>limit(read(a0, a1), a1, conditional(read(a0, a2), write(a0, a2, add(cos(a2), write(a0, a2, add(cos(sin(read(a0, protectedLog(abs(sub(a2, sin(a2))))))), add(a2, add(cos(0), a2))))))))</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>-1099.66</v>
+      </c>
+      <c r="C12" t="n">
+        <v>-1168.67</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-1149.75</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-1169.24</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-1267.78</v>
+      </c>
+      <c r="G12" t="n">
+        <v>-1387.27</v>
+      </c>
+      <c r="H12" t="n">
+        <v>-1480.57</v>
+      </c>
+      <c r="I12" t="n">
+        <v>-1460.15</v>
+      </c>
+      <c r="J12" t="n">
+        <v>-1178.4</v>
+      </c>
+      <c r="K12" t="n">
+        <v>-555.6</v>
+      </c>
+      <c r="L12" t="n">
+        <v>-1223.32</v>
+      </c>
+      <c r="M12" t="n">
+        <v>-1442.37</v>
+      </c>
+      <c r="N12" t="n">
+        <v>-1673.58</v>
+      </c>
+      <c r="O12" t="n">
+        <v>-1782.93</v>
+      </c>
+      <c r="P12" t="n">
+        <v>-1874.49</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>-1958.91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
write results to memory_grav
</commit_message>
<xml_diff>
--- a/pendulum/work_on_memory/memory_grav.xlsx
+++ b/pendulum/work_on_memory/memory_grav.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" tabRatio="600" firstSheet="0" activeTab="8" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="9.81" sheetId="1" state="visible" r:id="rId1"/>
@@ -11,6 +11,10 @@
     <sheet name="13" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="14" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="11" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="12" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="15" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="16" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="17" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -4668,4 +4672,2335 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>memProtectedDiv(limit(0, add(conditional(protectedLog(a2), a2), add(limit(sin(a2), add(limit(0, cos(a1), a2), add(a2, read(a0, a2))), a1), read(a0, a1))), a1), protectedLog(memProtectedDiv(read(a0, sub(abs(sub(abs(a2), 0)), add(a2, a1))), write(a0, a1, a2))))</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>-1546.64</v>
+      </c>
+      <c r="C1" t="n">
+        <v>-1815.63</v>
+      </c>
+      <c r="D1" t="n">
+        <v>-2048.64</v>
+      </c>
+      <c r="E1" t="n">
+        <v>-1986.24</v>
+      </c>
+      <c r="F1" t="n">
+        <v>-2017.97</v>
+      </c>
+      <c r="G1" t="n">
+        <v>-1956.27</v>
+      </c>
+      <c r="H1" t="n">
+        <v>-1862.65</v>
+      </c>
+      <c r="I1" t="n">
+        <v>-1810.06</v>
+      </c>
+      <c r="J1" t="n">
+        <v>-1499.63</v>
+      </c>
+      <c r="K1" t="n">
+        <v>-1303.98</v>
+      </c>
+      <c r="L1" t="n">
+        <v>-687.91</v>
+      </c>
+      <c r="M1" t="n">
+        <v>-1529.74</v>
+      </c>
+      <c r="N1" t="n">
+        <v>-1680.01</v>
+      </c>
+      <c r="O1" t="n">
+        <v>-1800.02</v>
+      </c>
+      <c r="P1" t="n">
+        <v>-1910.97</v>
+      </c>
+      <c r="Q1" t="n">
+        <v>-1993.46</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>sub(conditional(read(a0, a2), write(a0, write(a0, cos(cos(a2)), a1), add(write(a0, add(write(a0, a1, 0), a1), add(a2, cos(0))), cos(add(abs(protectedLog(sin(a1))), a1))))), sin(conditional(protectedLog(add(a2, a2)), conditional(a1, 0))))</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-1304.16</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-1809.17</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-1923.33</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-1949.15</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-1924.46</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-1847.54</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-1805.72</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-1806.17</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-1601.74</v>
+      </c>
+      <c r="K2" t="n">
+        <v>-1311.96</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-323.97</v>
+      </c>
+      <c r="M2" t="n">
+        <v>-1253.36</v>
+      </c>
+      <c r="N2" t="n">
+        <v>-1553.86</v>
+      </c>
+      <c r="O2" t="n">
+        <v>-1674.48</v>
+      </c>
+      <c r="P2" t="n">
+        <v>-1827.76</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>-1908.61</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>sub(read(a0, 0), add(a1, add(write(a0, a2, memProtectedDiv(add(protectedLog(a2), a1), a2)), a1)))</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>-2036.15</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-2073.24</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-2017.78</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-1938.69</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-1809.78</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-1756.3</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-1798.13</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-1685.72</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-1502.35</v>
+      </c>
+      <c r="K3" t="n">
+        <v>-1437.29</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-610.17</v>
+      </c>
+      <c r="M3" t="n">
+        <v>-1218.83</v>
+      </c>
+      <c r="N3" t="n">
+        <v>-1744.38</v>
+      </c>
+      <c r="O3" t="n">
+        <v>-1831.58</v>
+      </c>
+      <c r="P3" t="n">
+        <v>-1932.21</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>-2035.39</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>sub(sub(read(a0, a2), cos(sin(a2))), write(a0, abs(protectedLog(protectedLog(memProtectedDiv(abs(a2), sin(a1))))), sub(a2, memProtectedDiv(abs(add(a1, a1)), a2))))</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>-1662.51</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-1916.05</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-2064.97</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-1980.66</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-1855.5</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-1898.6</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-1778.2</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-1696.87</v>
+      </c>
+      <c r="J4" t="n">
+        <v>-1431</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-1293.88</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-400.11</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-1476.16</v>
+      </c>
+      <c r="N4" t="n">
+        <v>-1702.3</v>
+      </c>
+      <c r="O4" t="n">
+        <v>-1822.33</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-1919.24</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>-1978.61</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>sub(sub(read(a0, 0), write(a0, limit(cos(add(cos(a1), cos(a1))), a1, write(a0, write(a0, limit(limit(limit(cos(a2), 0, limit(0, 0, a1)), a1, 0), sub(write(a0, 0, memProtectedDiv(a2, read(a0, a2))), cos(limit(a1, 0, a1))), a1), write(a0, a2, cos(sub(a2, a2)))), memProtectedDiv(a1, write(a0, memProtectedDiv(limit(0, cos(a1), limit(a1, a2, a2)), a2), limit(a2, 0, memProtectedDiv(conditional(a2, 0), a2)))))), memProtectedDiv(a2, cos(add(cos(a1), cos(a2)))))), limit(read(a0, sin(0)), sub(0, a1), a1))</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-594.71</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-841.73</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-967.3200000000001</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-1199.59</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-1286.79</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-1265.67</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-1335.13</v>
+      </c>
+      <c r="I5" t="n">
+        <v>-1286.94</v>
+      </c>
+      <c r="J5" t="n">
+        <v>-1034.33</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-505.8</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-263.14</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-1204.1</v>
+      </c>
+      <c r="N5" t="n">
+        <v>-1457.88</v>
+      </c>
+      <c r="O5" t="n">
+        <v>-1640.81</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-1737.91</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-1891.94</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>sub(memProtectedDiv(read(a0, 0), sub(abs(sin(read(a0, add(conditional(a1, memProtectedDiv(conditional(cos(0), add(a2, a2)), a2)), add(protectedLog(abs(read(a0, a1))), sub(cos(0), cos(a1))))))), abs(write(a0, a2, sin(add(a2, sin(a2))))))), a2)</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-95.66</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-90.11</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-70.68000000000001</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-121.65</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-683.78</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-584.13</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-461.73</v>
+      </c>
+      <c r="I6" t="n">
+        <v>-546.08</v>
+      </c>
+      <c r="J6" t="n">
+        <v>-358.98</v>
+      </c>
+      <c r="K6" t="n">
+        <v>-404.18</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-453.71</v>
+      </c>
+      <c r="M6" t="n">
+        <v>-713</v>
+      </c>
+      <c r="N6" t="n">
+        <v>-891.42</v>
+      </c>
+      <c r="O6" t="n">
+        <v>-1141.75</v>
+      </c>
+      <c r="P6" t="n">
+        <v>-1355.19</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>-1664.47</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>sub(conditional(write(a0, a1, read(a0, 0)), write(a0, a1, add(a2, cos(0)))), limit(a1, limit(a2, a2, 0), conditional(read(a0, limit(a1, 0, a1)), cos(memProtectedDiv(a2, a1)))))</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>-510.39</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-710.61</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-1065.41</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-1332.35</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-1326.22</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-1520.13</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-1481.53</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-1353.81</v>
+      </c>
+      <c r="J7" t="n">
+        <v>-1206.96</v>
+      </c>
+      <c r="K7" t="n">
+        <v>-1097.49</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-381.68</v>
+      </c>
+      <c r="M7" t="n">
+        <v>-1453.84</v>
+      </c>
+      <c r="N7" t="n">
+        <v>-1607.75</v>
+      </c>
+      <c r="O7" t="n">
+        <v>-1750.01</v>
+      </c>
+      <c r="P7" t="n">
+        <v>-1840.64</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>-1969.3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>sub(read(a0, limit(limit(0, a2, a2), a1, sin(memProtectedDiv(0, 0)))), write(a0, a2, memProtectedDiv(add(memProtectedDiv(a1, abs(read(a0, cos(abs(a1))))), sub(limit(add(0, a1), a1, 0), cos(abs(conditional(add(a1, abs(memProtectedDiv(a2, a1))), a2))))), a2)))</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-2150.2</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-2265.67</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-2242.04</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-2217.66</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-2191.41</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-2055.48</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-2002.72</v>
+      </c>
+      <c r="I8" t="n">
+        <v>-1928.45</v>
+      </c>
+      <c r="J8" t="n">
+        <v>-1686.85</v>
+      </c>
+      <c r="K8" t="n">
+        <v>-1504.35</v>
+      </c>
+      <c r="L8" t="n">
+        <v>-595.09</v>
+      </c>
+      <c r="M8" t="n">
+        <v>-1486.07</v>
+      </c>
+      <c r="N8" t="n">
+        <v>-1689.5</v>
+      </c>
+      <c r="O8" t="n">
+        <v>-1792.89</v>
+      </c>
+      <c r="P8" t="n">
+        <v>-1929.85</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>-1943.55</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>sub(sub(read(a0, a2), write(a0, 0, add(memProtectedDiv(a2, protectedLog(abs(a1))), add(memProtectedDiv(a2, protectedLog(abs(a1))), cos(a2))))), memProtectedDiv(a1, a2))</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-828.4400000000001</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-926.7</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-1044.45</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-1015.63</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-1191.39</v>
+      </c>
+      <c r="G9" t="n">
+        <v>-1028.4</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-1109.45</v>
+      </c>
+      <c r="I9" t="n">
+        <v>-958.8200000000001</v>
+      </c>
+      <c r="J9" t="n">
+        <v>-848.4400000000001</v>
+      </c>
+      <c r="K9" t="n">
+        <v>-278.16</v>
+      </c>
+      <c r="L9" t="n">
+        <v>-276.41</v>
+      </c>
+      <c r="M9" t="n">
+        <v>-1284.16</v>
+      </c>
+      <c r="N9" t="n">
+        <v>-1525.83</v>
+      </c>
+      <c r="O9" t="n">
+        <v>-1702.27</v>
+      </c>
+      <c r="P9" t="n">
+        <v>-1862.45</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>-1971.14</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>sub(a2, add(sub(limit(read(a0, memProtectedDiv(a2, a2)), sin(a2), write(a0, a1, memProtectedDiv(sub(a1, a2), a2))), protectedLog(a2)), write(a0, limit(memProtectedDiv(a1, 0), a1, a2), a2)))</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>-1108.67</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-1901.69</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-1916.76</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-1686.89</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-1731.82</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-1630.48</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-1736.71</v>
+      </c>
+      <c r="I10" t="n">
+        <v>-1597.27</v>
+      </c>
+      <c r="J10" t="n">
+        <v>-1532.64</v>
+      </c>
+      <c r="K10" t="n">
+        <v>-1295.27</v>
+      </c>
+      <c r="L10" t="n">
+        <v>-491.19</v>
+      </c>
+      <c r="M10" t="n">
+        <v>-1487.56</v>
+      </c>
+      <c r="N10" t="n">
+        <v>-1679.01</v>
+      </c>
+      <c r="O10" t="n">
+        <v>-1849.04</v>
+      </c>
+      <c r="P10" t="n">
+        <v>-1843.19</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>-1940</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>write(a0, a2, add(sin(sin(a2)), abs(conditional(read(a0, a2), memProtectedDiv(0, memProtectedDiv(a1, a1))))))</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>-2669.62</v>
+      </c>
+      <c r="C1" t="n">
+        <v>-2692.93</v>
+      </c>
+      <c r="D1" t="n">
+        <v>-2702.1</v>
+      </c>
+      <c r="E1" t="n">
+        <v>-2698.86</v>
+      </c>
+      <c r="F1" t="n">
+        <v>-2694.08</v>
+      </c>
+      <c r="G1" t="n">
+        <v>-2652.58</v>
+      </c>
+      <c r="H1" t="n">
+        <v>-2589.41</v>
+      </c>
+      <c r="I1" t="n">
+        <v>-2511.85</v>
+      </c>
+      <c r="J1" t="n">
+        <v>-2355.9</v>
+      </c>
+      <c r="K1" t="n">
+        <v>-2228.19</v>
+      </c>
+      <c r="L1" t="n">
+        <v>-2101.4</v>
+      </c>
+      <c r="M1" t="n">
+        <v>-1955.93</v>
+      </c>
+      <c r="N1" t="n">
+        <v>-1761.54</v>
+      </c>
+      <c r="O1" t="n">
+        <v>-1514</v>
+      </c>
+      <c r="P1" t="n">
+        <v>-1679.05</v>
+      </c>
+      <c r="Q1" t="n">
+        <v>-1907.53</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>sub(add(sub(0, a2), write(a0, a2, add(read(a0, conditional(add(conditional(sub(a1, a1), a1), a2), cos(cos(0)))), a2))), limit(add(a1, conditional(a2, a1)), a2, read(a0, a1)))</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-2066.33</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-2382.67</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-2661.11</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-2668.2</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-2670.83</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-2602.59</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-2548.95</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-2457.39</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-2271.23</v>
+      </c>
+      <c r="K2" t="n">
+        <v>-2112.1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-1974.45</v>
+      </c>
+      <c r="M2" t="n">
+        <v>-1786.8</v>
+      </c>
+      <c r="N2" t="n">
+        <v>-1546.48</v>
+      </c>
+      <c r="O2" t="n">
+        <v>-1145.63</v>
+      </c>
+      <c r="P2" t="n">
+        <v>-1533.62</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>-1791.06</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>sub(protectedLog(sub(a2, limit(sub(a2, a1), sin(read(a0, 0)), read(a0, add(sub(a2, a2), read(a0, memProtectedDiv(0, a1))))))), write(a0, 0, limit(conditional(a1, 0), write(a0, 0, a2), sin(a2))))</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>-990.01</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-2325.79</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-2497.52</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-2485.87</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-2443.88</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-2428.4</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-2296.06</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-2226.04</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-1997.54</v>
+      </c>
+      <c r="K3" t="n">
+        <v>-1850.42</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-1741.24</v>
+      </c>
+      <c r="M3" t="n">
+        <v>-1662.87</v>
+      </c>
+      <c r="N3" t="n">
+        <v>-1517.35</v>
+      </c>
+      <c r="O3" t="n">
+        <v>-655.5700000000001</v>
+      </c>
+      <c r="P3" t="n">
+        <v>-1528.54</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>-1748.61</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>write(a0, a2, add(limit(conditional(a2, read(a0, read(a0, sub(0, 0)))), a2, sin(a2)), read(a0, a2)))</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>-2768.43</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-2779.22</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-2785.07</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-2786.63</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-2786.45</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-2744.11</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-2688.27</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-2633.07</v>
+      </c>
+      <c r="J4" t="n">
+        <v>-2477.7</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-2365.06</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-2203.58</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-1993.55</v>
+      </c>
+      <c r="N4" t="n">
+        <v>-1753.19</v>
+      </c>
+      <c r="O4" t="n">
+        <v>-1386.24</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-1504.7</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>-1816.8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>write(a0, sin(protectedLog(abs(a1))), conditional(add(sin(sin(sin(sin(sin(sin(sin(a2))))))), abs(read(a0, cos(a2)))), a1))</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-2594.84</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-2687.24</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-2679.92</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-2678.04</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-2662.47</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-2639.07</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-2571.66</v>
+      </c>
+      <c r="I5" t="n">
+        <v>-2488.84</v>
+      </c>
+      <c r="J5" t="n">
+        <v>-2298.38</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-2170.44</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-2035.61</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-1892.53</v>
+      </c>
+      <c r="N5" t="n">
+        <v>-1706.75</v>
+      </c>
+      <c r="O5" t="n">
+        <v>-1395.44</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-1623.72</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-1922.47</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>sub(sub(sin(sub(read(a0, limit(memProtectedDiv(0, a2), limit(add(abs(a1), conditional(a2, 0)), abs(a1), sin(0)), 0)), a2)), a2), write(a0, 0, a2))</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-313.62</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-309.19</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-362.1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-908.15</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-1202.81</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-1360.69</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-1355.73</v>
+      </c>
+      <c r="I6" t="n">
+        <v>-1414.98</v>
+      </c>
+      <c r="J6" t="n">
+        <v>-1503.86</v>
+      </c>
+      <c r="K6" t="n">
+        <v>-1552.51</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-1627.7</v>
+      </c>
+      <c r="M6" t="n">
+        <v>-1699.9</v>
+      </c>
+      <c r="N6" t="n">
+        <v>-1635.23</v>
+      </c>
+      <c r="O6" t="n">
+        <v>-1476.01</v>
+      </c>
+      <c r="P6" t="n">
+        <v>-1812.63</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>-1872.27</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>write(a0, 0, add(read(a0, a1), limit(protectedLog(abs(a1)), a2, sub(a1, sin(read(a0, 0))))))</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>-2768.78</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-2772.01</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-2782.57</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-2780.06</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-2759.69</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-2728.16</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-2680.65</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-2620.15</v>
+      </c>
+      <c r="J7" t="n">
+        <v>-2450.83</v>
+      </c>
+      <c r="K7" t="n">
+        <v>-2328.97</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-2200.88</v>
+      </c>
+      <c r="M7" t="n">
+        <v>-2029.87</v>
+      </c>
+      <c r="N7" t="n">
+        <v>-1766.71</v>
+      </c>
+      <c r="O7" t="n">
+        <v>-1258.31</v>
+      </c>
+      <c r="P7" t="n">
+        <v>-1698.91</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>-1855.85</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>sub(read(a0, a2), limit(read(a0, add(a2, 0)), add(conditional(a2, 0), add(abs(write(a0, 0, add(add(a2, sin(read(a0, a1))), cos(sub(sub(sin(limit(a1, a2, a1)), a2), 0))))), a2)), memProtectedDiv(a2, cos(conditional(read(a0, 0), sub(a1, a1))))))</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-2033.69</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-1837.57</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-1688.03</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-1463.7</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-2382.57</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-2320.07</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-2295.99</v>
+      </c>
+      <c r="I8" t="n">
+        <v>-2253.61</v>
+      </c>
+      <c r="J8" t="n">
+        <v>-2105.16</v>
+      </c>
+      <c r="K8" t="n">
+        <v>-1989.23</v>
+      </c>
+      <c r="L8" t="n">
+        <v>-1876.39</v>
+      </c>
+      <c r="M8" t="n">
+        <v>-1754.23</v>
+      </c>
+      <c r="N8" t="n">
+        <v>-1571.6</v>
+      </c>
+      <c r="O8" t="n">
+        <v>-781.05</v>
+      </c>
+      <c r="P8" t="n">
+        <v>-1687.71</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>-1840.64</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>memProtectedDiv(a2, limit(a1, sub(read(a0, a2), a1), sub(protectedLog(sub(add(read(a0, read(a0, 0)), cos(protectedLog(sub(protectedLog(sin(a2)), a1)))), 0)), write(a0, a2, limit(abs(a2), a2, a1)))))</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-1236.34</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-1121.11</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-990.45</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-842.23</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-1498.55</v>
+      </c>
+      <c r="G9" t="n">
+        <v>-1570.96</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-1591.57</v>
+      </c>
+      <c r="I9" t="n">
+        <v>-1534.34</v>
+      </c>
+      <c r="J9" t="n">
+        <v>-1616.96</v>
+      </c>
+      <c r="K9" t="n">
+        <v>-1372.63</v>
+      </c>
+      <c r="L9" t="n">
+        <v>-1212.99</v>
+      </c>
+      <c r="M9" t="n">
+        <v>-1128.96</v>
+      </c>
+      <c r="N9" t="n">
+        <v>-339.64</v>
+      </c>
+      <c r="O9" t="n">
+        <v>-212.58</v>
+      </c>
+      <c r="P9" t="n">
+        <v>-322.55</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>-1486.18</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>sub(read(a0, a1), add(a2, add(a2, write(a0, add(a2, a2), add(add(a2, add(0, write(a0, a2, add(add(add(a2, write(a0, protectedLog(a2), add(add(a2, a2), sin(read(a0, a1))))), a2), sin(add(a2, memProtectedDiv(conditional(a2, 0), a2))))))), sin(add(a2, memProtectedDiv(conditional(a2, 0), a2))))))))</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>-75.84</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-90.65000000000001</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-93.02</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-377.04</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-1013.77</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-1219.62</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-1445.8</v>
+      </c>
+      <c r="I10" t="n">
+        <v>-1588.49</v>
+      </c>
+      <c r="J10" t="n">
+        <v>-1748.68</v>
+      </c>
+      <c r="K10" t="n">
+        <v>-1745.73</v>
+      </c>
+      <c r="L10" t="n">
+        <v>-1693.82</v>
+      </c>
+      <c r="M10" t="n">
+        <v>-1596.18</v>
+      </c>
+      <c r="N10" t="n">
+        <v>-1350.75</v>
+      </c>
+      <c r="O10" t="n">
+        <v>-639.71</v>
+      </c>
+      <c r="P10" t="n">
+        <v>-1510.16</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>-1691.25</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>sub(cos(limit(a2, read(a0, a2), memProtectedDiv(add(a1, sub(protectedLog(abs(a2)), memProtectedDiv(a2, limit(a2, a1, conditional(cos(memProtectedDiv(memProtectedDiv(a1, 0), 0)), a1))))), conditional(cos(a2), sin(abs(a1)))))), write(a0, add(sin(0), 0), a2))</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>-2048.59</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-2418.38</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-2436.81</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-2317.63</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-2417.89</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-2351.25</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-2330.15</v>
+      </c>
+      <c r="I11" t="n">
+        <v>-2237.83</v>
+      </c>
+      <c r="J11" t="n">
+        <v>-2057.93</v>
+      </c>
+      <c r="K11" t="n">
+        <v>-1888.11</v>
+      </c>
+      <c r="L11" t="n">
+        <v>-1835.36</v>
+      </c>
+      <c r="M11" t="n">
+        <v>-1721.73</v>
+      </c>
+      <c r="N11" t="n">
+        <v>-1556.27</v>
+      </c>
+      <c r="O11" t="n">
+        <v>-506.41</v>
+      </c>
+      <c r="P11" t="n">
+        <v>-1664.24</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>-1815.41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>read(a0, write(a0, sub(a1, sin(a1)), add(add(read(a0, a1), conditional(conditional(sub(a1, sin(a1)), a1), read(a0, a2))), a2)))</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>-2768.35</v>
+      </c>
+      <c r="C1" t="n">
+        <v>-2786.37</v>
+      </c>
+      <c r="D1" t="n">
+        <v>-2793.93</v>
+      </c>
+      <c r="E1" t="n">
+        <v>-2795.54</v>
+      </c>
+      <c r="F1" t="n">
+        <v>-2781.8</v>
+      </c>
+      <c r="G1" t="n">
+        <v>-2744.76</v>
+      </c>
+      <c r="H1" t="n">
+        <v>-2691.61</v>
+      </c>
+      <c r="I1" t="n">
+        <v>-2631.82</v>
+      </c>
+      <c r="J1" t="n">
+        <v>-2488.31</v>
+      </c>
+      <c r="K1" t="n">
+        <v>-2385.77</v>
+      </c>
+      <c r="L1" t="n">
+        <v>-2259.19</v>
+      </c>
+      <c r="M1" t="n">
+        <v>-2140.6</v>
+      </c>
+      <c r="N1" t="n">
+        <v>-1986.84</v>
+      </c>
+      <c r="O1" t="n">
+        <v>-1775.66</v>
+      </c>
+      <c r="P1" t="n">
+        <v>-1338.45</v>
+      </c>
+      <c r="Q1" t="n">
+        <v>-1808.33</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>sub(sub(write(a0, a1, abs(add(read(a0, 0), a2))), add(a2, sub(cos(a1), a1))), a2)</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-2736.8</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-2731.22</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-2734.92</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-2730.01</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-2729.76</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-2685.54</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-2621.99</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-2551.45</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-2407.1</v>
+      </c>
+      <c r="K2" t="n">
+        <v>-2282.89</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-2172.35</v>
+      </c>
+      <c r="M2" t="n">
+        <v>-2047.36</v>
+      </c>
+      <c r="N2" t="n">
+        <v>-1884.95</v>
+      </c>
+      <c r="O2" t="n">
+        <v>-1674.58</v>
+      </c>
+      <c r="P2" t="n">
+        <v>-1191.12</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>-1755.34</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>sub(sub(write(a0, a2, sub(sub(sub(a1, limit(0, a2, read(a0, 0))), a2), add(conditional(a1, read(a0, 0)), cos(0)))), a2), sub(sin(memProtectedDiv(a1, a2)), limit(add(a2, a1), read(a0, a1), abs(write(a0, a1, a1)))))</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>-1231.08</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-1240.47</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-1405.93</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-1525.49</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-1757.85</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-2104.68</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-2079.97</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-2130.94</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-2154.2</v>
+      </c>
+      <c r="K3" t="n">
+        <v>-2021.62</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-2008.16</v>
+      </c>
+      <c r="M3" t="n">
+        <v>-1892.2</v>
+      </c>
+      <c r="N3" t="n">
+        <v>-1800.03</v>
+      </c>
+      <c r="O3" t="n">
+        <v>-1575.21</v>
+      </c>
+      <c r="P3" t="n">
+        <v>-1031.09</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>-1715.83</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>sub(sub(read(a0, a1), a2), add(a2, add(memProtectedDiv(abs(a2), memProtectedDiv(a2, a1)), write(a0, sub(add(add(0, a1), add(0, abs(limit(0, limit(0, read(a0, memProtectedDiv(a1, 0)), cos(a2)), a2)))), limit(limit(limit(sub(abs(0), add(add(add(limit(protectedLog(conditional(a1, a2)), a2, sin(limit(a1, a1, 0))), a2), a2), a2)), sub(memProtectedDiv(0, 0), a2), 0), 0, 0), a2, a2)), add(a2, sub(a2, sub(abs(add(a2, sub(a2, conditional(cos(a1), 0)))), add(add(add(a2, a2), a2), a2))))))))</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>-117.95</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-122.12</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-330.97</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-693.3</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-1146.7</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-1282.71</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-1351.14</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-1508.73</v>
+      </c>
+      <c r="J4" t="n">
+        <v>-1714.14</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-1689.34</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-1620.33</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-1552.07</v>
+      </c>
+      <c r="N4" t="n">
+        <v>-1412.79</v>
+      </c>
+      <c r="O4" t="n">
+        <v>-1214.99</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-440.83</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>-1499.32</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>write(a0, limit(abs(a2), add(0, read(a0, a1)), cos(0)), abs(add(conditional(read(a0, conditional(a1, a1)), sub(sin(read(a0, a1)), limit(a1, 0, a2))), a2)))</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-2670.23</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-2715.41</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-2709.5</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-2709.97</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-2684.9</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-2664.16</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-2591.44</v>
+      </c>
+      <c r="I5" t="n">
+        <v>-2524.07</v>
+      </c>
+      <c r="J5" t="n">
+        <v>-2385.62</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-2279.87</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-2182.7</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-2063.92</v>
+      </c>
+      <c r="N5" t="n">
+        <v>-1929</v>
+      </c>
+      <c r="O5" t="n">
+        <v>-1746.34</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-1352.97</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-1814.49</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>write(a0, protectedLog(0), add(a2, add(memProtectedDiv(conditional(a1, 0), read(a0, cos(read(a0, a2)))), add(a2, add(memProtectedDiv(conditional(a2, 0), a2), read(a0, 0))))))</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-2770.3</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-2790.36</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-2788.34</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-2799.26</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-2787.56</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-2742.47</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-2686.02</v>
+      </c>
+      <c r="I6" t="n">
+        <v>-2634.51</v>
+      </c>
+      <c r="J6" t="n">
+        <v>-2485.23</v>
+      </c>
+      <c r="K6" t="n">
+        <v>-2372.75</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-2249.86</v>
+      </c>
+      <c r="M6" t="n">
+        <v>-2116.39</v>
+      </c>
+      <c r="N6" t="n">
+        <v>-1950.47</v>
+      </c>
+      <c r="O6" t="n">
+        <v>-1766.08</v>
+      </c>
+      <c r="P6" t="n">
+        <v>-1339.49</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>-1758.76</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>add(write(a0, abs(add(0, a1)), add(a2, read(a0, 0))), abs(memProtectedDiv(add(a1, write(a0, limit(abs(a2), 0, 0), add(a2, read(a0, sin(abs(0)))))), sin(limit(a1, 0, sin(limit(0, 0, a2)))))))</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>-2681.15</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-2675.1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-2692.62</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-2676.98</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-2663.11</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-2663.25</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-2599.54</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-2518.03</v>
+      </c>
+      <c r="J7" t="n">
+        <v>-2349.95</v>
+      </c>
+      <c r="K7" t="n">
+        <v>-2202.63</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-2067.36</v>
+      </c>
+      <c r="M7" t="n">
+        <v>-1912.72</v>
+      </c>
+      <c r="N7" t="n">
+        <v>-1746.19</v>
+      </c>
+      <c r="O7" t="n">
+        <v>-1521.85</v>
+      </c>
+      <c r="P7" t="n">
+        <v>-1066.96</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>-1587.85</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>add(cos(limit(a2, a1, memProtectedDiv(write(a0, a1, protectedLog(sub(a2, read(a0, add(a1, a2))))), cos(a1)))), sub(abs(limit(protectedLog(cos(0)), add(a1, read(a0, protectedLog(conditional(a2, read(a0, 0))))), sin(write(a0, conditional(0, 0), a2)))), sin(a2)))</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-2425.37</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-2609.24</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-2607.23</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-2511.44</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-2491.33</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-2487.73</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-2472.83</v>
+      </c>
+      <c r="I8" t="n">
+        <v>-2412.97</v>
+      </c>
+      <c r="J8" t="n">
+        <v>-2246.1</v>
+      </c>
+      <c r="K8" t="n">
+        <v>-2138.74</v>
+      </c>
+      <c r="L8" t="n">
+        <v>-2046.81</v>
+      </c>
+      <c r="M8" t="n">
+        <v>-1919.08</v>
+      </c>
+      <c r="N8" t="n">
+        <v>-1780.9</v>
+      </c>
+      <c r="O8" t="n">
+        <v>-1605.14</v>
+      </c>
+      <c r="P8" t="n">
+        <v>-951.29</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>-1739.71</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>sub(read(a0, 0), memProtectedDiv(conditional(memProtectedDiv(cos(a1), read(a0, a1)), a1), limit(a2, a2, limit(read(a0, 0), write(a0, 0, cos(write(a0, a2, a1))), a1))))</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-1467.68</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-1381.36</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-1240.04</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-1215.76</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-1349.85</v>
+      </c>
+      <c r="G9" t="n">
+        <v>-1890.22</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-1782.25</v>
+      </c>
+      <c r="I9" t="n">
+        <v>-1489.9</v>
+      </c>
+      <c r="J9" t="n">
+        <v>-1659.7</v>
+      </c>
+      <c r="K9" t="n">
+        <v>-1563.07</v>
+      </c>
+      <c r="L9" t="n">
+        <v>-1396.78</v>
+      </c>
+      <c r="M9" t="n">
+        <v>-1395.53</v>
+      </c>
+      <c r="N9" t="n">
+        <v>-1130.52</v>
+      </c>
+      <c r="O9" t="n">
+        <v>-456.43</v>
+      </c>
+      <c r="P9" t="n">
+        <v>-444.02</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>-1568</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>abs(memProtectedDiv(cos(sub(protectedLog(a2), sin(a2))), add(limit(memProtectedDiv(memProtectedDiv(sin(memProtectedDiv(read(a0, read(a0, a1)), sin(memProtectedDiv(a2, a2)))), a2), a2), memProtectedDiv(read(a0, a2), a2), limit(read(a0, a2), write(a0, a1, a2), conditional(memProtectedDiv(a2, a1), a1))), a2)))</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>-2718.02</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-2713.97</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-2693.86</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-2617.65</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-2485.32</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-2500.34</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-2448.4</v>
+      </c>
+      <c r="I10" t="n">
+        <v>-2389.35</v>
+      </c>
+      <c r="J10" t="n">
+        <v>-2195.01</v>
+      </c>
+      <c r="K10" t="n">
+        <v>-2105.12</v>
+      </c>
+      <c r="L10" t="n">
+        <v>-2018.41</v>
+      </c>
+      <c r="M10" t="n">
+        <v>-1922.43</v>
+      </c>
+      <c r="N10" t="n">
+        <v>-1810.88</v>
+      </c>
+      <c r="O10" t="n">
+        <v>-1645.66</v>
+      </c>
+      <c r="P10" t="n">
+        <v>-1241.66</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>-1790.18</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>sub(cos(memProtectedDiv(read(a0, conditional(memProtectedDiv(a2, protectedLog(sin(a2))), protectedLog(memProtectedDiv(sub(a1, a2), sin(memProtectedDiv(sin(a2), 0)))))), limit(0, 0, write(a0, limit(a1, a2, memProtectedDiv(protectedLog(sub(a2, conditional(a2, a2))), sub(conditional(write(a0, a1, a1), write(a0, 0, a1)), conditional(memProtectedDiv(a2, a1), sub(a2, a1))))), memProtectedDiv(protectedLog(a2), a2))))), add(limit(abs(read(a0, a1)), 0, a1), a2))</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>-1531.79</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-2037.42</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-2219.12</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-2233.03</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-2107.07</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-2170.01</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-2112.64</v>
+      </c>
+      <c r="I11" t="n">
+        <v>-2101.62</v>
+      </c>
+      <c r="J11" t="n">
+        <v>-2124.16</v>
+      </c>
+      <c r="K11" t="n">
+        <v>-2036.25</v>
+      </c>
+      <c r="L11" t="n">
+        <v>-1984.24</v>
+      </c>
+      <c r="M11" t="n">
+        <v>-1903.17</v>
+      </c>
+      <c r="N11" t="n">
+        <v>-1824.26</v>
+      </c>
+      <c r="O11" t="n">
+        <v>-1715.01</v>
+      </c>
+      <c r="P11" t="n">
+        <v>-1441.36</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>-1863.87</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>write(a0, 0, add(read(a0, a2), memProtectedDiv(sin(a2), abs(memProtectedDiv(cos(sin(a2)), limit(limit(0, a1, cos(read(a0, 0))), cos(read(a0, 0)), a1))))))</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>-2767.73</v>
+      </c>
+      <c r="C12" t="n">
+        <v>-2778.29</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-2777.48</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-2785.03</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-2779.95</v>
+      </c>
+      <c r="G12" t="n">
+        <v>-2735.87</v>
+      </c>
+      <c r="H12" t="n">
+        <v>-2686.2</v>
+      </c>
+      <c r="I12" t="n">
+        <v>-2610.15</v>
+      </c>
+      <c r="J12" t="n">
+        <v>-2441.83</v>
+      </c>
+      <c r="K12" t="n">
+        <v>-2273.33</v>
+      </c>
+      <c r="L12" t="n">
+        <v>-2172.54</v>
+      </c>
+      <c r="M12" t="n">
+        <v>-2128.74</v>
+      </c>
+      <c r="N12" t="n">
+        <v>-2004.35</v>
+      </c>
+      <c r="O12" t="n">
+        <v>-1795.16</v>
+      </c>
+      <c r="P12" t="n">
+        <v>-1206.17</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>-1744.28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>write(a0, add(a1, a2), add(limit(a1, memProtectedDiv(limit(a1, cos(0), add(add(0, sub(a2, a1)), cos(a2))), read(a0, sub(a1, 0))), sub(a2, a1)), add(a2, read(a0, sub(0, 0)))))</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>-2764.36</v>
+      </c>
+      <c r="C1" t="n">
+        <v>-2748.18</v>
+      </c>
+      <c r="D1" t="n">
+        <v>-2758.68</v>
+      </c>
+      <c r="E1" t="n">
+        <v>-2764.52</v>
+      </c>
+      <c r="F1" t="n">
+        <v>-2742.38</v>
+      </c>
+      <c r="G1" t="n">
+        <v>-2686.6</v>
+      </c>
+      <c r="H1" t="n">
+        <v>-2612.3</v>
+      </c>
+      <c r="I1" t="n">
+        <v>-2540.18</v>
+      </c>
+      <c r="J1" t="n">
+        <v>-2370.62</v>
+      </c>
+      <c r="K1" t="n">
+        <v>-2281.97</v>
+      </c>
+      <c r="L1" t="n">
+        <v>-2149.84</v>
+      </c>
+      <c r="M1" t="n">
+        <v>-2073.19</v>
+      </c>
+      <c r="N1" t="n">
+        <v>-1986.31</v>
+      </c>
+      <c r="O1" t="n">
+        <v>-1864.02</v>
+      </c>
+      <c r="P1" t="n">
+        <v>-1674.8</v>
+      </c>
+      <c r="Q1" t="n">
+        <v>-1814.51</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>write(a0, a1, add(read(a0, a1), sub(a2, limit(memProtectedDiv(read(a0, limit(add(a1, abs(a1)), 0, a1)), a2), sin(0), sub(0, a2)))))</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-2787.02</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-2798.14</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-2801.23</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-2811.9</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-2796.74</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-2757.48</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-2697.66</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-2636.08</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-2491.69</v>
+      </c>
+      <c r="K2" t="n">
+        <v>-2384.04</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-2262.66</v>
+      </c>
+      <c r="M2" t="n">
+        <v>-2148.01</v>
+      </c>
+      <c r="N2" t="n">
+        <v>-2000.2</v>
+      </c>
+      <c r="O2" t="n">
+        <v>-1800.05</v>
+      </c>
+      <c r="P2" t="n">
+        <v>-1503.02</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>-1666.32</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>write(a0, sub(conditional(a2, memProtectedDiv(0, 0)), 0), add(a2, add(add(a2, read(a0, abs(abs(a2)))), limit(a2, sin(sin(a1)), limit(limit(protectedLog(0), sin(sin(a1)), limit(0, read(a0, 0), sin(sub(0, add(a2, a1))))), read(a0, a2), sin(sub(0, cos(sub(limit(a1, read(a0, a1), a1), a1)))))))))</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>-2786.23</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-2794.71</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-2800.4</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-2803.53</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-2795.32</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-2750.48</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-2695.18</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-2627.58</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-2480</v>
+      </c>
+      <c r="K3" t="n">
+        <v>-2372.37</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-2257.89</v>
+      </c>
+      <c r="M3" t="n">
+        <v>-2142.43</v>
+      </c>
+      <c r="N3" t="n">
+        <v>-2040.04</v>
+      </c>
+      <c r="O3" t="n">
+        <v>-1770.54</v>
+      </c>
+      <c r="P3" t="n">
+        <v>-1673.97</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>-1791.71</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>sub(write(a0, a2, add(a2, read(a0, a2))), add(add(a2, add(memProtectedDiv(0, cos(a2)), memProtectedDiv(a2, sub(cos(a2), a1)))), a2))</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>-1799.19</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-1912.49</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-2025.43</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-2259.05</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-2331.64</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-2348.13</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-2288.58</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-2299.05</v>
+      </c>
+      <c r="J4" t="n">
+        <v>-2217.46</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-2107.71</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-2018.41</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-1892.87</v>
+      </c>
+      <c r="N4" t="n">
+        <v>-1760.54</v>
+      </c>
+      <c r="O4" t="n">
+        <v>-1527.14</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-1249.42</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>-1478.6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>sub(write(a0, a1, add(read(a0, cos(cos(sub(a2, abs(abs(a2)))))), a2)), memProtectedDiv(limit(a1, 0, abs(a1)), sub(a2, sin(a2))))</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-1857.36</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-1948.2</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-2133.51</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-2141.45</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-2310.07</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-2494.17</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-2412.06</v>
+      </c>
+      <c r="I5" t="n">
+        <v>-2365.16</v>
+      </c>
+      <c r="J5" t="n">
+        <v>-2158.75</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-2078.62</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-1988.58</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-1917.14</v>
+      </c>
+      <c r="N5" t="n">
+        <v>-1759.05</v>
+      </c>
+      <c r="O5" t="n">
+        <v>-1547.07</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-1232.37</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-1484.07</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>write(a0, a2, add(add(limit(limit(read(a0, cos(abs(memProtectedDiv(a1, cos(0))))), 0, a1), a2, add(a2, a2)), add(a2, protectedLog(protectedLog(add(read(a0, a1), protectedLog(read(a0, sub(a2, a2)))))))), read(a0, limit(a1, protectedLog(read(a0, a1)), add(conditional(a2, memProtectedDiv(a1, a1)), 0)))))</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-2795.95</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-2787.73</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-2795.32</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-2798.84</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-2795.54</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-2758.92</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-2700.98</v>
+      </c>
+      <c r="I6" t="n">
+        <v>-2639.74</v>
+      </c>
+      <c r="J6" t="n">
+        <v>-2493.57</v>
+      </c>
+      <c r="K6" t="n">
+        <v>-2385.53</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-2266.11</v>
+      </c>
+      <c r="M6" t="n">
+        <v>-2152.08</v>
+      </c>
+      <c r="N6" t="n">
+        <v>-2006.26</v>
+      </c>
+      <c r="O6" t="n">
+        <v>-1807.17</v>
+      </c>
+      <c r="P6" t="n">
+        <v>-1494.16</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>-1662.88</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>write(a0, a2, add(read(a0, a2), add(add(add(a2, add(a2, limit(conditional(a2, read(a0, a1)), a2, 0))), add(a2, limit(conditional(a2, read(a0, 0)), a2, 0))), add(a2, limit(conditional(a2, read(a0, 0)), a2, 0)))))</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>-2799.49</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-2792.46</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-2793.29</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-2809.5</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-2796.65</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-2759.27</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-2700.41</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-2641.18</v>
+      </c>
+      <c r="J7" t="n">
+        <v>-2497.48</v>
+      </c>
+      <c r="K7" t="n">
+        <v>-2391.43</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-2263.32</v>
+      </c>
+      <c r="M7" t="n">
+        <v>-2151.5</v>
+      </c>
+      <c r="N7" t="n">
+        <v>-2005.09</v>
+      </c>
+      <c r="O7" t="n">
+        <v>-1802.83</v>
+      </c>
+      <c r="P7" t="n">
+        <v>-1497.44</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>-1617.48</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>sub(0, add(add(limit(read(a0, sub(cos(sub(0, a2)), conditional(sin(0), a1))), a2, protectedLog(add(write(a0, limit(0, 0, limit(read(a0, a1), a2, read(a0, a1))), sin(a2)), conditional(a2, 0)))), add(abs(sub(cos(protectedLog(a2)), a1)), a2)), read(a0, 0)))</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-249.58</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-209.67</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-148.21</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-192.6</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-942.51</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-1010.41</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-963.04</v>
+      </c>
+      <c r="I8" t="n">
+        <v>-1007.31</v>
+      </c>
+      <c r="J8" t="n">
+        <v>-1008.82</v>
+      </c>
+      <c r="K8" t="n">
+        <v>-1146.4</v>
+      </c>
+      <c r="L8" t="n">
+        <v>-1225.41</v>
+      </c>
+      <c r="M8" t="n">
+        <v>-1207.8</v>
+      </c>
+      <c r="N8" t="n">
+        <v>-1172.6</v>
+      </c>
+      <c r="O8" t="n">
+        <v>-1139.61</v>
+      </c>
+      <c r="P8" t="n">
+        <v>-889.92</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>-1478.63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
complete set up for random grav testing
</commit_message>
<xml_diff>
--- a/pendulum/work_on_memory/memory_grav.xlsx
+++ b/pendulum/work_on_memory/memory_grav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sky/Documents/Work Info/Research Assistant/deap_experiments/pendulum/work_on_memory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3615C1-F7F5-D34F-A9AC-21ECCA524148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D279759-1B6F-3142-B91B-BB2362958275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15620" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Outliers" sheetId="2" r:id="rId1"/>
@@ -17433,15 +17433,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>641350</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>128270</xdr:rowOff>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -20192,7 +20192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12340CC-15ED-8D45-A66A-77A6A53E1180}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="81" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScale="81" workbookViewId="0">
       <selection activeCell="V40" sqref="V40"/>
     </sheetView>
   </sheetViews>
@@ -23850,8 +23850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>